<commit_message>
school lisitng by danish
updated school list
</commit_message>
<xml_diff>
--- a/data/school listing.xlsx
+++ b/data/school listing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8160e739ff5d14cf/Documents/GitHub/grp-the-r-ones/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\grp-the-r-ones\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{772530E7-A491-4D94-BFF5-F6EE3CB176B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{969A0B65-4F16-4849-9E0C-067723D51892}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52CB8078-77CF-45E2-AD5C-05707D51A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5A9532B9-1078-4A7A-974D-4A0853E75333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A9532B9-1078-4A7A-974D-4A0853E75333}"/>
   </bookViews>
   <sheets>
     <sheet name="school listing" sheetId="9" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1811" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="546">
   <si>
     <r>
       <rPr>
@@ -2473,17 +2473,181 @@
   <si>
     <t>4.925969501368837, 114.96535117976734</t>
   </si>
+  <si>
+    <t>4.596426022570256, 114.33174024999532</t>
+  </si>
+  <si>
+    <t>4.681075184100253, 114.49495629351502</t>
+  </si>
+  <si>
+    <t>4.653305838698077, 114.43888138187674</t>
+  </si>
+  <si>
+    <t>4.588597312130063, 114.1787611260574</t>
+  </si>
+  <si>
+    <t>4.6093643546865115, 114.33113906838526</t>
+  </si>
+  <si>
+    <t>4.581462088991996, 114.20560061946712</t>
+  </si>
+  <si>
+    <t>4.588484273324178, 114.22931559536826</t>
+  </si>
+  <si>
+    <t>4.589226189753305, 114.24218055674653</t>
+  </si>
+  <si>
+    <t>4.765105430311369, 114.81077309722116</t>
+  </si>
+  <si>
+    <t>4.905314344088125, 114.91078013954879</t>
+  </si>
+  <si>
+    <t>4.941287018454734, 114.88027842605744</t>
+  </si>
+  <si>
+    <t>4.995976047287888, 114.9774815972213</t>
+  </si>
+  <si>
+    <t>4.947163105491392, 114.95278105489348</t>
+  </si>
+  <si>
+    <t>4.905008865107954, 114.9330764125657</t>
+  </si>
+  <si>
+    <t>4.972910829412266, 114.89394853954889</t>
+  </si>
+  <si>
+    <t>4.906157264702269, 114.91246532791058</t>
+  </si>
+  <si>
+    <t>4.977517920656551, 114.89996411256583</t>
+  </si>
+  <si>
+    <t>4.579131903669992, 114.20525296242745</t>
+  </si>
+  <si>
+    <t>4.599915657780337, 114.32169202885574</t>
+  </si>
+  <si>
+    <t>4.873486796103531, 114.89901355674658</t>
+  </si>
+  <si>
+    <t>4.928676959254864, 114.96261509536822</t>
+  </si>
+  <si>
+    <t>4.88610433117746, 114.86170176653202</t>
+  </si>
+  <si>
+    <t>4.987379699862789, 115.0203412194466</t>
+  </si>
+  <si>
+    <t>4.895490505663748, 114.9253765743357</t>
+  </si>
+  <si>
+    <t>4.925680779356876, 114.90722972605745</t>
+  </si>
+  <si>
+    <t>4.906047270537197, 114.9390955702381</t>
+  </si>
+  <si>
+    <t>4.907181674826401, 114.90172624088189</t>
+  </si>
+  <si>
+    <t>4.900565528960677, 114.90040239536809</t>
+  </si>
+  <si>
+    <t>4.96095445432593, 114.97269053164956</t>
+  </si>
+  <si>
+    <t>4.951035615926786, 114.95575212420428</t>
+  </si>
+  <si>
+    <t>4.895284099427465, 114.9317107260574</t>
+  </si>
+  <si>
+    <t>4.995312144828727, 115.02335412605741</t>
+  </si>
+  <si>
+    <t>4.876564195478929, 114.85083241022548</t>
+  </si>
+  <si>
+    <t>4.92562757155879, 114.96282474325517</t>
+  </si>
+  <si>
+    <t>4.992016201152402, 114.94776349234152</t>
+  </si>
+  <si>
+    <t>4.9067428211416315, 114.83666459228056</t>
+  </si>
+  <si>
+    <t>4.977643816017232, 114.98605374325503</t>
+  </si>
+  <si>
+    <t>4.88343370197034, 114.85575885674669</t>
+  </si>
+  <si>
+    <t>5.025148134552888, 115.04387276890513</t>
+  </si>
+  <si>
+    <t>4.938473618099268, 114.94212720833951</t>
+  </si>
+  <si>
+    <t>4.946968328109143, 114.96481995622658</t>
+  </si>
+  <si>
+    <t>4.935585785593987, 114.90657481256582</t>
+  </si>
+  <si>
+    <t>4.948365083172124, 114.95916722420434</t>
+  </si>
+  <si>
+    <t>4.958955511990044, 114.94071011071273</t>
+  </si>
+  <si>
+    <t>4.935432019970616, 114.94880514510791</t>
+  </si>
+  <si>
+    <t>4.847926085798664, 114.84359257849611</t>
+  </si>
+  <si>
+    <t>4.910523153628393, 114.98858033298237</t>
+  </si>
+  <si>
+    <t>4.894036297053241, 114.84767399907436</t>
+  </si>
+  <si>
+    <t>4.940849549473641, 114.96403735775058</t>
+  </si>
+  <si>
+    <t>4.924259594545598, 114.83408620149314</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2736,267 +2900,269 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="12"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="10"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3713,20 +3879,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED54A88-6810-4FBE-8CDE-8EA5829FFAA6}">
   <dimension ref="A1:J253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B144" sqref="B144"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H87" sqref="H86:H87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.796875" style="40" customWidth="1"/>
-    <col min="2" max="2" width="68.19921875" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="8.8984375" style="40" customWidth="1"/>
-    <col min="8" max="8" width="37.796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.8984375" style="40"/>
+    <col min="1" max="1" width="3.83203125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="8.83203125" style="40" customWidth="1"/>
+    <col min="8" max="8" width="63.33203125" style="40" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="40" t="s">
         <v>396</v>
       </c>
@@ -3758,7 +3924,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="40">
         <v>1</v>
       </c>
@@ -3790,7 +3956,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="40">
         <v>2</v>
       </c>
@@ -3819,7 +3985,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="40">
         <v>3</v>
       </c>
@@ -3848,7 +4014,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="40">
         <v>6</v>
       </c>
@@ -3877,7 +4043,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="40">
         <v>10</v>
       </c>
@@ -3906,7 +4072,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="40">
         <v>14</v>
       </c>
@@ -3935,7 +4101,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="40">
         <v>15</v>
       </c>
@@ -3967,7 +4133,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="40">
         <v>19</v>
       </c>
@@ -3996,7 +4162,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="40">
         <v>20</v>
       </c>
@@ -4025,7 +4191,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="40">
         <v>21</v>
       </c>
@@ -4054,7 +4220,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" s="40">
         <v>22</v>
       </c>
@@ -4086,7 +4252,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" s="40">
         <v>23</v>
       </c>
@@ -4115,7 +4281,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" s="40">
         <v>26</v>
       </c>
@@ -4147,7 +4313,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" s="40">
         <v>30</v>
       </c>
@@ -4176,7 +4342,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" s="40">
         <v>32</v>
       </c>
@@ -4205,7 +4371,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="40">
         <v>33</v>
       </c>
@@ -4234,7 +4400,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="40">
         <v>37</v>
       </c>
@@ -4263,7 +4429,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="40">
         <v>39</v>
       </c>
@@ -4292,7 +4458,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="40">
         <v>40</v>
       </c>
@@ -4321,7 +4487,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="40">
         <v>43</v>
       </c>
@@ -4350,7 +4516,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="40">
         <v>45</v>
       </c>
@@ -4379,7 +4545,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="40">
         <v>54</v>
       </c>
@@ -4408,7 +4574,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="40">
         <v>55</v>
       </c>
@@ -4437,7 +4603,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="40">
         <v>58</v>
       </c>
@@ -4466,7 +4632,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="40">
         <v>62</v>
       </c>
@@ -4495,7 +4661,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="40">
         <v>64</v>
       </c>
@@ -4524,7 +4690,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="40">
         <v>65</v>
       </c>
@@ -4553,7 +4719,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="40">
         <v>66</v>
       </c>
@@ -4582,7 +4748,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="40">
         <v>67</v>
       </c>
@@ -4611,7 +4777,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="40">
         <v>73</v>
       </c>
@@ -4640,7 +4806,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="40">
         <v>77</v>
       </c>
@@ -4669,7 +4835,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="40">
         <v>78</v>
       </c>
@@ -4698,7 +4864,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="40">
         <v>79</v>
       </c>
@@ -4724,7 +4890,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="40">
         <v>80</v>
       </c>
@@ -4750,7 +4916,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="40">
         <v>82</v>
       </c>
@@ -4776,7 +4942,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="40">
         <v>83</v>
       </c>
@@ -4802,7 +4968,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="40">
         <v>84</v>
       </c>
@@ -4828,7 +4994,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="40">
         <v>87</v>
       </c>
@@ -4854,7 +5020,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="40">
         <v>88</v>
       </c>
@@ -4880,7 +5046,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="40">
         <v>89</v>
       </c>
@@ -4906,7 +5072,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="40">
         <v>90</v>
       </c>
@@ -4932,7 +5098,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="40">
         <v>91</v>
       </c>
@@ -4958,7 +5124,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="40">
         <v>92</v>
       </c>
@@ -4984,7 +5150,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="40">
         <v>93</v>
       </c>
@@ -5010,7 +5176,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="40">
         <v>94</v>
       </c>
@@ -5036,7 +5202,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="40">
         <v>96</v>
       </c>
@@ -5062,7 +5228,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="40">
         <v>98</v>
       </c>
@@ -5088,7 +5254,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="40">
         <v>99</v>
       </c>
@@ -5114,7 +5280,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="40">
         <v>100</v>
       </c>
@@ -5140,7 +5306,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="40">
         <v>101</v>
       </c>
@@ -5166,7 +5332,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="40">
         <v>102</v>
       </c>
@@ -5192,7 +5358,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="40">
         <v>103</v>
       </c>
@@ -5218,7 +5384,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="40">
         <v>104</v>
       </c>
@@ -5244,7 +5410,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="40">
         <v>105</v>
       </c>
@@ -5270,7 +5436,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9">
       <c r="A56" s="40">
         <v>106</v>
       </c>
@@ -5296,7 +5462,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9">
       <c r="A57" s="40">
         <v>107</v>
       </c>
@@ -5322,7 +5488,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="40">
         <v>110</v>
       </c>
@@ -5348,7 +5514,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="40">
         <v>111</v>
       </c>
@@ -5374,7 +5540,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9">
       <c r="A60" s="40">
         <v>113</v>
       </c>
@@ -5400,7 +5566,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9">
       <c r="A61" s="40">
         <v>114</v>
       </c>
@@ -5426,7 +5592,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9">
       <c r="A62" s="40">
         <v>115</v>
       </c>
@@ -5452,7 +5618,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9">
       <c r="A63" s="40">
         <v>116</v>
       </c>
@@ -5478,7 +5644,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9">
       <c r="A64" s="40">
         <v>117</v>
       </c>
@@ -5504,7 +5670,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="40">
         <v>118</v>
       </c>
@@ -5530,7 +5696,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="40">
         <v>119</v>
       </c>
@@ -5556,7 +5722,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9">
       <c r="A67" s="40">
         <v>120</v>
       </c>
@@ -5582,7 +5748,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9">
       <c r="A68" s="40">
         <v>121</v>
       </c>
@@ -5608,7 +5774,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9">
       <c r="A69" s="40">
         <v>123</v>
       </c>
@@ -5634,7 +5800,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9">
       <c r="A70" s="40">
         <v>124</v>
       </c>
@@ -5660,7 +5826,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="A71" s="40">
         <v>127</v>
       </c>
@@ -5686,7 +5852,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="A72" s="40">
         <v>128</v>
       </c>
@@ -5712,7 +5878,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9">
       <c r="A73" s="40">
         <v>129</v>
       </c>
@@ -5738,7 +5904,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="A74" s="40">
         <v>133</v>
       </c>
@@ -5764,7 +5930,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="A75" s="40">
         <v>134</v>
       </c>
@@ -5790,7 +5956,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="A76" s="40">
         <v>136</v>
       </c>
@@ -5816,7 +5982,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9">
       <c r="A77" s="40">
         <v>138</v>
       </c>
@@ -5842,7 +6008,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9">
       <c r="A78" s="40">
         <v>139</v>
       </c>
@@ -5868,7 +6034,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9">
       <c r="A79" s="40">
         <v>140</v>
       </c>
@@ -5894,7 +6060,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="A80" s="40">
         <v>141</v>
       </c>
@@ -5920,7 +6086,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9">
       <c r="A81" s="40">
         <v>142</v>
       </c>
@@ -5946,7 +6112,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9">
       <c r="A82" s="40">
         <v>143</v>
       </c>
@@ -5972,7 +6138,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9">
       <c r="A83" s="40">
         <v>144</v>
       </c>
@@ -5998,11 +6164,11 @@
         <v>440</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9">
       <c r="A84" s="40">
         <v>145</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="43" t="s">
         <v>278</v>
       </c>
       <c r="C84" s="40" t="s">
@@ -6020,15 +6186,18 @@
       <c r="G84" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H84" s="40" t="s">
+        <v>496</v>
+      </c>
       <c r="I84" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9">
       <c r="A85" s="40">
         <v>146</v>
       </c>
-      <c r="B85" s="40" t="s">
+      <c r="B85" s="43" t="s">
         <v>279</v>
       </c>
       <c r="C85" s="40" t="s">
@@ -6046,15 +6215,18 @@
       <c r="G85" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H85" s="40" t="s">
+        <v>497</v>
+      </c>
       <c r="I85" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9">
       <c r="A86" s="40">
         <v>147</v>
       </c>
-      <c r="B86" s="40" t="s">
+      <c r="B86" s="43" t="s">
         <v>280</v>
       </c>
       <c r="C86" s="40" t="s">
@@ -6072,15 +6244,18 @@
       <c r="G86" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H86" s="40" t="s">
+        <v>498</v>
+      </c>
       <c r="I86" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9">
       <c r="A87" s="40">
         <v>148</v>
       </c>
-      <c r="B87" s="40" t="s">
+      <c r="B87" s="43" t="s">
         <v>281</v>
       </c>
       <c r="C87" s="40" t="s">
@@ -6098,15 +6273,18 @@
       <c r="G87" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H87" s="43" t="s">
+        <v>499</v>
+      </c>
       <c r="I87" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9">
       <c r="A88" s="40">
         <v>149</v>
       </c>
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="43" t="s">
         <v>282</v>
       </c>
       <c r="C88" s="40" t="s">
@@ -6124,15 +6302,18 @@
       <c r="G88" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H88" s="40" t="s">
+        <v>500</v>
+      </c>
       <c r="I88" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9">
       <c r="A89" s="40">
         <v>151</v>
       </c>
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="43" t="s">
         <v>284</v>
       </c>
       <c r="C89" s="40" t="s">
@@ -6150,15 +6331,18 @@
       <c r="G89" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H89" s="40" t="s">
+        <v>501</v>
+      </c>
       <c r="I89" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9">
       <c r="A90" s="40">
         <v>152</v>
       </c>
-      <c r="B90" s="40" t="s">
+      <c r="B90" s="43" t="s">
         <v>285</v>
       </c>
       <c r="C90" s="40" t="s">
@@ -6176,15 +6360,18 @@
       <c r="G90" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H90" s="40" t="s">
+        <v>502</v>
+      </c>
       <c r="I90" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9">
       <c r="A91" s="40">
         <v>153</v>
       </c>
-      <c r="B91" s="40" t="s">
+      <c r="B91" s="43" t="s">
         <v>286</v>
       </c>
       <c r="C91" s="40" t="s">
@@ -6202,15 +6389,18 @@
       <c r="G91" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H91" s="40" t="s">
+        <v>503</v>
+      </c>
       <c r="I91" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9">
       <c r="A92" s="40">
         <v>154</v>
       </c>
-      <c r="B92" s="40" t="s">
+      <c r="B92" s="43" t="s">
         <v>288</v>
       </c>
       <c r="C92" s="40" t="s">
@@ -6228,15 +6418,18 @@
       <c r="G92" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H92" s="40" t="s">
+        <v>504</v>
+      </c>
       <c r="I92" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9">
       <c r="A93" s="40">
         <v>155</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="43" t="s">
         <v>289</v>
       </c>
       <c r="C93" s="40" t="s">
@@ -6254,15 +6447,18 @@
       <c r="G93" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H93" s="40" t="s">
+        <v>505</v>
+      </c>
       <c r="I93" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9">
       <c r="A94" s="40">
         <v>156</v>
       </c>
-      <c r="B94" s="40" t="s">
+      <c r="B94" s="43" t="s">
         <v>290</v>
       </c>
       <c r="C94" s="40" t="s">
@@ -6280,15 +6476,18 @@
       <c r="G94" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H94" s="40" t="s">
+        <v>506</v>
+      </c>
       <c r="I94" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9">
       <c r="A95" s="40">
         <v>157</v>
       </c>
-      <c r="B95" s="40" t="s">
+      <c r="B95" s="43" t="s">
         <v>291</v>
       </c>
       <c r="C95" s="40" t="s">
@@ -6306,15 +6505,18 @@
       <c r="G95" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H95" s="40" t="s">
+        <v>507</v>
+      </c>
       <c r="I95" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9">
       <c r="A96" s="40">
         <v>158</v>
       </c>
-      <c r="B96" s="40" t="s">
+      <c r="B96" s="43" t="s">
         <v>292</v>
       </c>
       <c r="C96" s="40" t="s">
@@ -6332,15 +6534,18 @@
       <c r="G96" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H96" s="40" t="s">
+        <v>508</v>
+      </c>
       <c r="I96" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9">
       <c r="A97" s="40">
         <v>159</v>
       </c>
-      <c r="B97" s="40" t="s">
+      <c r="B97" s="43" t="s">
         <v>294</v>
       </c>
       <c r="C97" s="40" t="s">
@@ -6358,15 +6563,18 @@
       <c r="G97" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H97" s="40" t="s">
+        <v>509</v>
+      </c>
       <c r="I97" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9">
       <c r="A98" s="40">
         <v>160</v>
       </c>
-      <c r="B98" s="40" t="s">
+      <c r="B98" s="43" t="s">
         <v>295</v>
       </c>
       <c r="C98" s="40" t="s">
@@ -6384,15 +6592,18 @@
       <c r="G98" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H98" s="40" t="s">
+        <v>510</v>
+      </c>
       <c r="I98" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9">
       <c r="A99" s="40">
         <v>161</v>
       </c>
-      <c r="B99" s="40" t="s">
+      <c r="B99" s="43" t="s">
         <v>296</v>
       </c>
       <c r="C99" s="40" t="s">
@@ -6410,15 +6621,18 @@
       <c r="G99" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H99" s="40" t="s">
+        <v>511</v>
+      </c>
       <c r="I99" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9">
       <c r="A100" s="40">
         <v>162</v>
       </c>
-      <c r="B100" s="40" t="s">
+      <c r="B100" s="43" t="s">
         <v>297</v>
       </c>
       <c r="C100" s="40" t="s">
@@ -6436,15 +6650,18 @@
       <c r="G100" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H100" s="40" t="s">
+        <v>512</v>
+      </c>
       <c r="I100" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9">
       <c r="A101" s="40">
         <v>163</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="43" t="s">
         <v>298</v>
       </c>
       <c r="C101" s="40" t="s">
@@ -6462,15 +6679,18 @@
       <c r="G101" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H101" s="40" t="s">
+        <v>513</v>
+      </c>
       <c r="I101" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9">
       <c r="A102" s="40">
         <v>164</v>
       </c>
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="43" t="s">
         <v>299</v>
       </c>
       <c r="C102" s="40" t="s">
@@ -6488,15 +6708,18 @@
       <c r="G102" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H102" s="40" t="s">
+        <v>514</v>
+      </c>
       <c r="I102" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9">
       <c r="A103" s="40">
         <v>165</v>
       </c>
-      <c r="B103" s="40" t="s">
+      <c r="B103" s="43" t="s">
         <v>301</v>
       </c>
       <c r="C103" s="40" t="s">
@@ -6514,15 +6737,18 @@
       <c r="G103" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H103" s="40" t="s">
+        <v>515</v>
+      </c>
       <c r="I103" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9">
       <c r="A104" s="40">
         <v>166</v>
       </c>
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="43" t="s">
         <v>302</v>
       </c>
       <c r="C104" s="40" t="s">
@@ -6540,15 +6766,18 @@
       <c r="G104" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H104" s="40" t="s">
+        <v>516</v>
+      </c>
       <c r="I104" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9">
       <c r="A105" s="40">
         <v>167</v>
       </c>
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="43" t="s">
         <v>303</v>
       </c>
       <c r="C105" s="40" t="s">
@@ -6566,15 +6795,18 @@
       <c r="G105" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H105" s="40" t="s">
+        <v>517</v>
+      </c>
       <c r="I105" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9">
       <c r="A106" s="40">
         <v>168</v>
       </c>
-      <c r="B106" s="40" t="s">
+      <c r="B106" s="43" t="s">
         <v>304</v>
       </c>
       <c r="C106" s="40" t="s">
@@ -6592,15 +6824,18 @@
       <c r="G106" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H106" s="40" t="s">
+        <v>518</v>
+      </c>
       <c r="I106" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9">
       <c r="A107" s="40">
         <v>169</v>
       </c>
-      <c r="B107" s="40" t="s">
+      <c r="B107" s="43" t="s">
         <v>305</v>
       </c>
       <c r="C107" s="40" t="s">
@@ -6618,15 +6853,18 @@
       <c r="G107" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H107" s="40" t="s">
+        <v>519</v>
+      </c>
       <c r="I107" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9">
       <c r="A108" s="40">
         <v>170</v>
       </c>
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="43" t="s">
         <v>306</v>
       </c>
       <c r="C108" s="40" t="s">
@@ -6644,15 +6882,18 @@
       <c r="G108" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H108" s="40" t="s">
+        <v>520</v>
+      </c>
       <c r="I108" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9">
       <c r="A109" s="40">
         <v>171</v>
       </c>
-      <c r="B109" s="40" t="s">
+      <c r="B109" s="43" t="s">
         <v>307</v>
       </c>
       <c r="C109" s="40" t="s">
@@ -6670,15 +6911,18 @@
       <c r="G109" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H109" s="40" t="s">
+        <v>521</v>
+      </c>
       <c r="I109" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9">
       <c r="A110" s="40">
         <v>172</v>
       </c>
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="43" t="s">
         <v>308</v>
       </c>
       <c r="C110" s="40" t="s">
@@ -6696,15 +6940,18 @@
       <c r="G110" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H110" s="40" t="s">
+        <v>522</v>
+      </c>
       <c r="I110" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9">
       <c r="A111" s="40">
         <v>173</v>
       </c>
-      <c r="B111" s="40" t="s">
+      <c r="B111" s="43" t="s">
         <v>309</v>
       </c>
       <c r="C111" s="40" t="s">
@@ -6722,15 +6969,18 @@
       <c r="G111" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H111" s="40" t="s">
+        <v>523</v>
+      </c>
       <c r="I111" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9">
       <c r="A112" s="40">
         <v>174</v>
       </c>
-      <c r="B112" s="40" t="s">
+      <c r="B112" s="43" t="s">
         <v>310</v>
       </c>
       <c r="C112" s="40" t="s">
@@ -6748,15 +6998,18 @@
       <c r="G112" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H112" s="43" t="s">
+        <v>524</v>
+      </c>
       <c r="I112" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9">
       <c r="A113" s="40">
         <v>175</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="43" t="s">
         <v>311</v>
       </c>
       <c r="C113" s="40" t="s">
@@ -6774,15 +7027,18 @@
       <c r="G113" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H113" s="44" t="s">
+        <v>545</v>
+      </c>
       <c r="I113" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9">
       <c r="A114" s="40">
         <v>176</v>
       </c>
-      <c r="B114" s="40" t="s">
+      <c r="B114" s="43" t="s">
         <v>312</v>
       </c>
       <c r="C114" s="40" t="s">
@@ -6800,15 +7056,18 @@
       <c r="G114" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H114" s="40" t="s">
+        <v>525</v>
+      </c>
       <c r="I114" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9">
       <c r="A115" s="40">
         <v>177</v>
       </c>
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="43" t="s">
         <v>313</v>
       </c>
       <c r="C115" s="40" t="s">
@@ -6826,15 +7085,18 @@
       <c r="G115" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H115" s="43" t="s">
+        <v>526</v>
+      </c>
       <c r="I115" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9">
       <c r="A116" s="40">
         <v>178</v>
       </c>
-      <c r="B116" s="40" t="s">
+      <c r="B116" s="43" t="s">
         <v>314</v>
       </c>
       <c r="C116" s="40" t="s">
@@ -6852,15 +7114,18 @@
       <c r="G116" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H116" s="40" t="s">
+        <v>527</v>
+      </c>
       <c r="I116" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9">
       <c r="A117" s="40">
         <v>179</v>
       </c>
-      <c r="B117" s="40" t="s">
+      <c r="B117" s="43" t="s">
         <v>315</v>
       </c>
       <c r="C117" s="40" t="s">
@@ -6878,15 +7143,18 @@
       <c r="G117" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H117" s="40" t="s">
+        <v>528</v>
+      </c>
       <c r="I117" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9">
       <c r="A118" s="40">
         <v>180</v>
       </c>
-      <c r="B118" s="40" t="s">
+      <c r="B118" s="43" t="s">
         <v>316</v>
       </c>
       <c r="C118" s="40" t="s">
@@ -6904,15 +7172,18 @@
       <c r="G118" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H118" s="40" t="s">
+        <v>529</v>
+      </c>
       <c r="I118" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9">
       <c r="A119" s="40">
         <v>181</v>
       </c>
-      <c r="B119" s="40" t="s">
+      <c r="B119" s="43" t="s">
         <v>317</v>
       </c>
       <c r="C119" s="40" t="s">
@@ -6930,15 +7201,18 @@
       <c r="G119" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H119" s="40" t="s">
+        <v>530</v>
+      </c>
       <c r="I119" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9">
       <c r="A120" s="40">
         <v>182</v>
       </c>
-      <c r="B120" s="40" t="s">
+      <c r="B120" s="43" t="s">
         <v>318</v>
       </c>
       <c r="C120" s="40" t="s">
@@ -6956,15 +7230,18 @@
       <c r="G120" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H120" s="40" t="s">
+        <v>531</v>
+      </c>
       <c r="I120" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9">
       <c r="A121" s="40">
         <v>183</v>
       </c>
-      <c r="B121" s="40" t="s">
+      <c r="B121" s="43" t="s">
         <v>319</v>
       </c>
       <c r="C121" s="40" t="s">
@@ -6982,15 +7259,18 @@
       <c r="G121" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H121" s="40" t="s">
+        <v>532</v>
+      </c>
       <c r="I121" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9">
       <c r="A122" s="40">
         <v>184</v>
       </c>
-      <c r="B122" s="40" t="s">
+      <c r="B122" s="43" t="s">
         <v>320</v>
       </c>
       <c r="C122" s="40" t="s">
@@ -7008,15 +7288,18 @@
       <c r="G122" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H122" s="40" t="s">
+        <v>533</v>
+      </c>
       <c r="I122" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9">
       <c r="A123" s="40">
         <v>185</v>
       </c>
-      <c r="B123" s="40" t="s">
+      <c r="B123" s="43" t="s">
         <v>321</v>
       </c>
       <c r="C123" s="40" t="s">
@@ -7034,15 +7317,18 @@
       <c r="G123" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H123" s="40" t="s">
+        <v>534</v>
+      </c>
       <c r="I123" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9">
       <c r="A124" s="40">
         <v>186</v>
       </c>
-      <c r="B124" s="40" t="s">
+      <c r="B124" s="43" t="s">
         <v>322</v>
       </c>
       <c r="C124" s="40" t="s">
@@ -7060,15 +7346,18 @@
       <c r="G124" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H124" s="40" t="s">
+        <v>535</v>
+      </c>
       <c r="I124" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9">
       <c r="A125" s="40">
         <v>187</v>
       </c>
-      <c r="B125" s="40" t="s">
+      <c r="B125" s="43" t="s">
         <v>323</v>
       </c>
       <c r="C125" s="40" t="s">
@@ -7086,15 +7375,18 @@
       <c r="G125" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H125" s="40" t="s">
+        <v>536</v>
+      </c>
       <c r="I125" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9">
       <c r="A126" s="40">
         <v>188</v>
       </c>
-      <c r="B126" s="40" t="s">
+      <c r="B126" s="43" t="s">
         <v>324</v>
       </c>
       <c r="C126" s="40" t="s">
@@ -7112,15 +7404,18 @@
       <c r="G126" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H126" s="40" t="s">
+        <v>537</v>
+      </c>
       <c r="I126" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9">
       <c r="A127" s="40">
         <v>189</v>
       </c>
-      <c r="B127" s="40" t="s">
+      <c r="B127" s="43" t="s">
         <v>325</v>
       </c>
       <c r="C127" s="40" t="s">
@@ -7138,15 +7433,18 @@
       <c r="G127" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H127" s="40" t="s">
+        <v>538</v>
+      </c>
       <c r="I127" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9">
       <c r="A128" s="40">
         <v>190</v>
       </c>
-      <c r="B128" s="40" t="s">
+      <c r="B128" s="43" t="s">
         <v>326</v>
       </c>
       <c r="C128" s="40" t="s">
@@ -7164,15 +7462,18 @@
       <c r="G128" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H128" s="40" t="s">
+        <v>539</v>
+      </c>
       <c r="I128" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9">
       <c r="A129" s="40">
         <v>191</v>
       </c>
-      <c r="B129" s="40" t="s">
+      <c r="B129" s="43" t="s">
         <v>327</v>
       </c>
       <c r="C129" s="40" t="s">
@@ -7190,15 +7491,18 @@
       <c r="G129" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H129" s="40" t="s">
+        <v>540</v>
+      </c>
       <c r="I129" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9">
       <c r="A130" s="40">
         <v>192</v>
       </c>
-      <c r="B130" s="40" t="s">
+      <c r="B130" s="43" t="s">
         <v>328</v>
       </c>
       <c r="C130" s="40" t="s">
@@ -7216,11 +7520,14 @@
       <c r="G130" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H130" s="43" t="s">
+        <v>541</v>
+      </c>
       <c r="I130" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9">
       <c r="A131" s="40">
         <v>193</v>
       </c>
@@ -7242,15 +7549,18 @@
       <c r="G131" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H131" s="40" t="s">
+        <v>542</v>
+      </c>
       <c r="I131" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9">
       <c r="A132" s="40">
         <v>195</v>
       </c>
-      <c r="B132" s="40" t="s">
+      <c r="B132" s="43" t="s">
         <v>331</v>
       </c>
       <c r="C132" s="40" t="s">
@@ -7268,15 +7578,18 @@
       <c r="G132" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H132" s="40" t="s">
+        <v>543</v>
+      </c>
       <c r="I132" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9">
       <c r="A133" s="40">
         <v>196</v>
       </c>
-      <c r="B133" s="40" t="s">
+      <c r="B133" s="43" t="s">
         <v>332</v>
       </c>
       <c r="C133" s="40" t="s">
@@ -7294,11 +7607,14 @@
       <c r="G133" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="H133" s="40" t="s">
+        <v>544</v>
+      </c>
       <c r="I133" s="40" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9">
       <c r="A134" s="40">
         <v>197</v>
       </c>
@@ -7327,7 +7643,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9">
       <c r="A135" s="40">
         <v>198</v>
       </c>
@@ -7356,7 +7672,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9">
       <c r="A136" s="40">
         <v>199</v>
       </c>
@@ -7385,7 +7701,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9">
       <c r="A137" s="40">
         <v>200</v>
       </c>
@@ -7414,7 +7730,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9">
       <c r="A138" s="40">
         <v>201</v>
       </c>
@@ -7443,7 +7759,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9">
       <c r="A139" s="40">
         <v>202</v>
       </c>
@@ -7472,7 +7788,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9">
       <c r="A140" s="40">
         <v>203</v>
       </c>
@@ -7501,7 +7817,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9">
       <c r="A141" s="40">
         <v>204</v>
       </c>
@@ -7530,7 +7846,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9">
       <c r="A142" s="40">
         <v>206</v>
       </c>
@@ -7559,7 +7875,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9">
       <c r="A143" s="40">
         <v>207</v>
       </c>
@@ -7588,7 +7904,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9">
       <c r="A144" s="40">
         <v>208</v>
       </c>
@@ -7617,7 +7933,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9">
       <c r="A145" s="40">
         <v>209</v>
       </c>
@@ -7639,18 +7955,18 @@
       <c r="G145" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H145" s="87" t="s">
+      <c r="H145" s="42" t="s">
         <v>495</v>
       </c>
       <c r="I145" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9">
       <c r="A146" s="40">
         <v>211</v>
       </c>
-      <c r="B146" s="87" t="s">
+      <c r="B146" s="42" t="s">
         <v>349</v>
       </c>
       <c r="C146" s="40" t="s">
@@ -7668,18 +7984,18 @@
       <c r="G146" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H146" s="87" t="s">
+      <c r="H146" s="42" t="s">
         <v>458</v>
       </c>
       <c r="I146" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9">
       <c r="A147" s="40">
         <v>212</v>
       </c>
-      <c r="B147" s="87" t="s">
+      <c r="B147" s="42" t="s">
         <v>351</v>
       </c>
       <c r="C147" s="40" t="s">
@@ -7697,18 +8013,18 @@
       <c r="G147" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H147" s="87" t="s">
+      <c r="H147" s="42" t="s">
         <v>461</v>
       </c>
       <c r="I147" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9">
       <c r="A148" s="40">
         <v>213</v>
       </c>
-      <c r="B148" s="87" t="s">
+      <c r="B148" s="42" t="s">
         <v>353</v>
       </c>
       <c r="C148" s="40" t="s">
@@ -7726,18 +8042,18 @@
       <c r="G148" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H148" s="87" t="s">
+      <c r="H148" s="42" t="s">
         <v>460</v>
       </c>
       <c r="I148" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9">
       <c r="A149" s="40">
         <v>214</v>
       </c>
-      <c r="B149" s="87" t="s">
+      <c r="B149" s="42" t="s">
         <v>354</v>
       </c>
       <c r="C149" s="40" t="s">
@@ -7755,18 +8071,18 @@
       <c r="G149" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H149" s="87" t="s">
+      <c r="H149" s="42" t="s">
         <v>459</v>
       </c>
       <c r="I149" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9">
       <c r="A150" s="40">
         <v>215</v>
       </c>
-      <c r="B150" s="87" t="s">
+      <c r="B150" s="42" t="s">
         <v>356</v>
       </c>
       <c r="C150" s="40" t="s">
@@ -7784,18 +8100,18 @@
       <c r="G150" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H150" s="87" t="s">
+      <c r="H150" s="42" t="s">
         <v>462</v>
       </c>
       <c r="I150" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9">
       <c r="A151" s="40">
         <v>216</v>
       </c>
-      <c r="B151" s="87" t="s">
+      <c r="B151" s="42" t="s">
         <v>357</v>
       </c>
       <c r="C151" s="40" t="s">
@@ -7813,18 +8129,18 @@
       <c r="G151" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H151" s="87" t="s">
+      <c r="H151" s="42" t="s">
         <v>463</v>
       </c>
       <c r="I151" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9">
       <c r="A152" s="40">
         <v>218</v>
       </c>
-      <c r="B152" s="87" t="s">
+      <c r="B152" s="42" t="s">
         <v>359</v>
       </c>
       <c r="C152" s="40" t="s">
@@ -7842,18 +8158,18 @@
       <c r="G152" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H152" s="87" t="s">
+      <c r="H152" s="42" t="s">
         <v>464</v>
       </c>
       <c r="I152" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9">
       <c r="A153" s="40">
         <v>219</v>
       </c>
-      <c r="B153" s="87" t="s">
+      <c r="B153" s="42" t="s">
         <v>360</v>
       </c>
       <c r="C153" s="40" t="s">
@@ -7871,18 +8187,18 @@
       <c r="G153" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H153" s="87" t="s">
+      <c r="H153" s="42" t="s">
         <v>465</v>
       </c>
       <c r="I153" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9">
       <c r="A154" s="40">
         <v>220</v>
       </c>
-      <c r="B154" s="87" t="s">
+      <c r="B154" s="42" t="s">
         <v>361</v>
       </c>
       <c r="C154" s="40" t="s">
@@ -7900,18 +8216,18 @@
       <c r="G154" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H154" s="87" t="s">
+      <c r="H154" s="42" t="s">
         <v>466</v>
       </c>
       <c r="I154" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9">
       <c r="A155" s="40">
         <v>221</v>
       </c>
-      <c r="B155" s="87" t="s">
+      <c r="B155" s="42" t="s">
         <v>362</v>
       </c>
       <c r="C155" s="40" t="s">
@@ -7929,18 +8245,18 @@
       <c r="G155" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H155" s="87" t="s">
+      <c r="H155" s="42" t="s">
         <v>494</v>
       </c>
       <c r="I155" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9">
       <c r="A156" s="40">
         <v>222</v>
       </c>
-      <c r="B156" s="87" t="s">
+      <c r="B156" s="42" t="s">
         <v>363</v>
       </c>
       <c r="C156" s="40" t="s">
@@ -7958,18 +8274,18 @@
       <c r="G156" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H156" s="87" t="s">
+      <c r="H156" s="42" t="s">
         <v>467</v>
       </c>
       <c r="I156" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9">
       <c r="A157" s="40">
         <v>223</v>
       </c>
-      <c r="B157" s="87" t="s">
+      <c r="B157" s="42" t="s">
         <v>364</v>
       </c>
       <c r="C157" s="40" t="s">
@@ -7987,18 +8303,18 @@
       <c r="G157" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H157" s="87" t="s">
+      <c r="H157" s="42" t="s">
         <v>468</v>
       </c>
       <c r="I157" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9">
       <c r="A158" s="40">
         <v>224</v>
       </c>
-      <c r="B158" s="87" t="s">
+      <c r="B158" s="42" t="s">
         <v>365</v>
       </c>
       <c r="C158" s="40" t="s">
@@ -8016,18 +8332,18 @@
       <c r="G158" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H158" s="87" t="s">
+      <c r="H158" s="42" t="s">
         <v>469</v>
       </c>
       <c r="I158" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9">
       <c r="A159" s="40">
         <v>225</v>
       </c>
-      <c r="B159" s="87" t="s">
+      <c r="B159" s="42" t="s">
         <v>366</v>
       </c>
       <c r="C159" s="40" t="s">
@@ -8045,18 +8361,18 @@
       <c r="G159" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H159" s="87" t="s">
+      <c r="H159" s="42" t="s">
         <v>470</v>
       </c>
       <c r="I159" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9">
       <c r="A160" s="40">
         <v>226</v>
       </c>
-      <c r="B160" s="87" t="s">
+      <c r="B160" s="42" t="s">
         <v>367</v>
       </c>
       <c r="C160" s="40" t="s">
@@ -8074,18 +8390,18 @@
       <c r="G160" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H160" s="87" t="s">
+      <c r="H160" s="42" t="s">
         <v>471</v>
       </c>
       <c r="I160" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9">
       <c r="A161" s="40">
         <v>227</v>
       </c>
-      <c r="B161" s="87" t="s">
+      <c r="B161" s="42" t="s">
         <v>368</v>
       </c>
       <c r="C161" s="40" t="s">
@@ -8103,18 +8419,18 @@
       <c r="G161" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H161" s="87" t="s">
+      <c r="H161" s="42" t="s">
         <v>472</v>
       </c>
       <c r="I161" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9">
       <c r="A162" s="40">
         <v>228</v>
       </c>
-      <c r="B162" s="87" t="s">
+      <c r="B162" s="42" t="s">
         <v>369</v>
       </c>
       <c r="C162" s="40" t="s">
@@ -8132,18 +8448,18 @@
       <c r="G162" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H162" s="87" t="s">
+      <c r="H162" s="42" t="s">
         <v>473</v>
       </c>
       <c r="I162" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9">
       <c r="A163" s="40">
         <v>229</v>
       </c>
-      <c r="B163" s="87" t="s">
+      <c r="B163" s="42" t="s">
         <v>370</v>
       </c>
       <c r="C163" s="40" t="s">
@@ -8161,18 +8477,18 @@
       <c r="G163" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H163" s="87" t="s">
+      <c r="H163" s="42" t="s">
         <v>474</v>
       </c>
       <c r="I163" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9">
       <c r="A164" s="40">
         <v>230</v>
       </c>
-      <c r="B164" s="87" t="s">
+      <c r="B164" s="42" t="s">
         <v>371</v>
       </c>
       <c r="C164" s="40" t="s">
@@ -8190,18 +8506,18 @@
       <c r="G164" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H164" s="87" t="s">
+      <c r="H164" s="42" t="s">
         <v>475</v>
       </c>
       <c r="I164" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9">
       <c r="A165" s="40">
         <v>233</v>
       </c>
-      <c r="B165" s="87" t="s">
+      <c r="B165" s="42" t="s">
         <v>374</v>
       </c>
       <c r="C165" s="40" t="s">
@@ -8219,18 +8535,18 @@
       <c r="G165" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H165" s="87" t="s">
+      <c r="H165" s="42" t="s">
         <v>476</v>
       </c>
       <c r="I165" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9">
       <c r="A166" s="40">
         <v>234</v>
       </c>
-      <c r="B166" s="87" t="s">
+      <c r="B166" s="42" t="s">
         <v>343</v>
       </c>
       <c r="C166" s="40" t="s">
@@ -8248,18 +8564,18 @@
       <c r="G166" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H166" s="87" t="s">
+      <c r="H166" s="42" t="s">
         <v>477</v>
       </c>
       <c r="I166" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9">
       <c r="A167" s="40">
         <v>235</v>
       </c>
-      <c r="B167" s="87" t="s">
+      <c r="B167" s="42" t="s">
         <v>375</v>
       </c>
       <c r="C167" s="40" t="s">
@@ -8277,18 +8593,18 @@
       <c r="G167" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H167" s="87" t="s">
+      <c r="H167" s="42" t="s">
         <v>478</v>
       </c>
       <c r="I167" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9">
       <c r="A168" s="40">
         <v>236</v>
       </c>
-      <c r="B168" s="87" t="s">
+      <c r="B168" s="42" t="s">
         <v>376</v>
       </c>
       <c r="C168" s="40" t="s">
@@ -8306,18 +8622,18 @@
       <c r="G168" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H168" s="87" t="s">
+      <c r="H168" s="42" t="s">
         <v>479</v>
       </c>
       <c r="I168" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9">
       <c r="A169" s="40">
         <v>237</v>
       </c>
-      <c r="B169" s="87" t="s">
+      <c r="B169" s="42" t="s">
         <v>377</v>
       </c>
       <c r="C169" s="40" t="s">
@@ -8335,14 +8651,14 @@
       <c r="G169" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H169" s="87" t="s">
+      <c r="H169" s="42" t="s">
         <v>480</v>
       </c>
       <c r="I169" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9">
       <c r="A170" s="40">
         <v>238</v>
       </c>
@@ -8371,7 +8687,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9">
       <c r="A171" s="40">
         <v>239</v>
       </c>
@@ -8393,18 +8709,18 @@
       <c r="G171" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H171" s="87" t="s">
+      <c r="H171" s="42" t="s">
         <v>482</v>
       </c>
       <c r="I171" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9">
       <c r="A172" s="40">
         <v>241</v>
       </c>
-      <c r="B172" s="87" t="s">
+      <c r="B172" s="42" t="s">
         <v>381</v>
       </c>
       <c r="C172" s="40" t="s">
@@ -8422,18 +8738,18 @@
       <c r="G172" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H172" s="87" t="s">
+      <c r="H172" s="42" t="s">
         <v>483</v>
       </c>
       <c r="I172" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9">
       <c r="A173" s="40">
         <v>242</v>
       </c>
-      <c r="B173" s="87" t="s">
+      <c r="B173" s="42" t="s">
         <v>382</v>
       </c>
       <c r="C173" s="40" t="s">
@@ -8451,18 +8767,18 @@
       <c r="G173" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H173" s="87" t="s">
+      <c r="H173" s="42" t="s">
         <v>484</v>
       </c>
       <c r="I173" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9">
       <c r="A174" s="40">
         <v>243</v>
       </c>
-      <c r="B174" s="87" t="s">
+      <c r="B174" s="42" t="s">
         <v>383</v>
       </c>
       <c r="C174" s="40" t="s">
@@ -8480,14 +8796,14 @@
       <c r="G174" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H174" s="87" t="s">
+      <c r="H174" s="42" t="s">
         <v>485</v>
       </c>
       <c r="I174" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9">
       <c r="A175" s="40">
         <v>244</v>
       </c>
@@ -8509,18 +8825,18 @@
       <c r="G175" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H175" s="87" t="s">
+      <c r="H175" s="42" t="s">
         <v>486</v>
       </c>
       <c r="I175" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9">
       <c r="A176" s="40">
         <v>245</v>
       </c>
-      <c r="B176" s="87" t="s">
+      <c r="B176" s="42" t="s">
         <v>385</v>
       </c>
       <c r="C176" s="40" t="s">
@@ -8538,18 +8854,18 @@
       <c r="G176" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H176" s="87" t="s">
+      <c r="H176" s="42" t="s">
         <v>487</v>
       </c>
       <c r="I176" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9">
       <c r="A177" s="40">
         <v>246</v>
       </c>
-      <c r="B177" s="87" t="s">
+      <c r="B177" s="42" t="s">
         <v>386</v>
       </c>
       <c r="C177" s="40" t="s">
@@ -8567,18 +8883,18 @@
       <c r="G177" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H177" s="87" t="s">
+      <c r="H177" s="42" t="s">
         <v>488</v>
       </c>
       <c r="I177" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9">
       <c r="A178" s="40">
         <v>247</v>
       </c>
-      <c r="B178" s="87" t="s">
+      <c r="B178" s="42" t="s">
         <v>387</v>
       </c>
       <c r="C178" s="40" t="s">
@@ -8596,18 +8912,18 @@
       <c r="G178" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H178" s="87" t="s">
+      <c r="H178" s="42" t="s">
         <v>489</v>
       </c>
       <c r="I178" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9">
       <c r="A179" s="40">
         <v>248</v>
       </c>
-      <c r="B179" s="87" t="s">
+      <c r="B179" s="42" t="s">
         <v>388</v>
       </c>
       <c r="C179" s="40" t="s">
@@ -8625,18 +8941,18 @@
       <c r="G179" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H179" s="87" t="s">
+      <c r="H179" s="42" t="s">
         <v>490</v>
       </c>
       <c r="I179" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9">
       <c r="A180" s="40">
         <v>249</v>
       </c>
-      <c r="B180" s="87" t="s">
+      <c r="B180" s="42" t="s">
         <v>389</v>
       </c>
       <c r="C180" s="40" t="s">
@@ -8654,18 +8970,18 @@
       <c r="G180" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H180" s="87" t="s">
+      <c r="H180" s="42" t="s">
         <v>491</v>
       </c>
       <c r="I180" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9">
       <c r="A181" s="40">
         <v>250</v>
       </c>
-      <c r="B181" s="87" t="s">
+      <c r="B181" s="42" t="s">
         <v>390</v>
       </c>
       <c r="C181" s="40" t="s">
@@ -8683,18 +8999,18 @@
       <c r="G181" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H181" s="87" t="s">
+      <c r="H181" s="42" t="s">
         <v>492</v>
       </c>
       <c r="I181" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9">
       <c r="A182" s="40">
         <v>252</v>
       </c>
-      <c r="B182" s="87" t="s">
+      <c r="B182" s="42" t="s">
         <v>395</v>
       </c>
       <c r="C182" s="40" t="s">
@@ -8712,14 +9028,14 @@
       <c r="G182" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H182" s="87" t="s">
+      <c r="H182" s="42" t="s">
         <v>493</v>
       </c>
       <c r="I182" s="40" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9">
       <c r="A183" s="40">
         <v>16</v>
       </c>
@@ -8742,7 +9058,7 @@
         <v>4.7643813772432102</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9">
       <c r="A184" s="40">
         <v>17</v>
       </c>
@@ -8765,7 +9081,7 @@
         <v>4.7303408612861197</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9">
       <c r="A185" s="40">
         <v>25</v>
       </c>
@@ -8788,7 +9104,7 @@
         <v>4.7122173305573503</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9">
       <c r="A186" s="40">
         <v>24</v>
       </c>
@@ -8811,7 +9127,7 @@
         <v>4.7092599719366799</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9">
       <c r="A187" s="40">
         <v>240</v>
       </c>
@@ -8834,7 +9150,7 @@
         <v>4.7026965754013998</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9">
       <c r="A188" s="40">
         <v>86</v>
       </c>
@@ -8857,7 +9173,7 @@
         <v>5.0209225218448896</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9">
       <c r="A189" s="40">
         <v>18</v>
       </c>
@@ -8880,7 +9196,7 @@
         <v>4.6984751109092997</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9">
       <c r="A190" s="40">
         <v>97</v>
       </c>
@@ -8903,7 +9219,7 @@
         <v>5.0360679337986802</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9">
       <c r="A191" s="40">
         <v>81</v>
       </c>
@@ -8926,7 +9242,7 @@
         <v>4.9725808072562501</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9">
       <c r="A192" s="40">
         <v>210</v>
       </c>
@@ -8949,7 +9265,7 @@
         <v>4.9623238674432102</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7">
       <c r="A193" s="40">
         <v>251</v>
       </c>
@@ -8972,7 +9288,7 @@
         <v>4.99217655509214</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7">
       <c r="A194" s="40">
         <v>69</v>
       </c>
@@ -8995,7 +9311,7 @@
         <v>4.8329781069781701</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7">
       <c r="A195" s="40">
         <v>72</v>
       </c>
@@ -9018,7 +9334,7 @@
         <v>4.9310816401703104</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7">
       <c r="A196" s="40">
         <v>56</v>
       </c>
@@ -9041,7 +9357,7 @@
         <v>4.9611573668001503</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7">
       <c r="A197" s="40">
         <v>59</v>
       </c>
@@ -9064,7 +9380,7 @@
         <v>4.9476103533575904</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7">
       <c r="A198" s="40">
         <v>7</v>
       </c>
@@ -9087,7 +9403,7 @@
         <v>4.87249923415777</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7">
       <c r="A199" s="40">
         <v>75</v>
       </c>
@@ -9110,7 +9426,7 @@
         <v>4.9295250645260502</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7">
       <c r="A200" s="40">
         <v>68</v>
       </c>
@@ -9133,7 +9449,7 @@
         <v>4.9325702172486201</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7">
       <c r="A201" s="40">
         <v>76</v>
       </c>
@@ -9156,7 +9472,7 @@
         <v>4.9470109997956904</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7">
       <c r="A202" s="40">
         <v>61</v>
       </c>
@@ -9179,7 +9495,7 @@
         <v>4.82309208955476</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7">
       <c r="A203" s="40">
         <v>232</v>
       </c>
@@ -9202,7 +9518,7 @@
         <v>4.9690740699832396</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7">
       <c r="A204" s="40">
         <v>74</v>
       </c>
@@ -9225,7 +9541,7 @@
         <v>4.8631400434660499</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7">
       <c r="A205" s="40">
         <v>53</v>
       </c>
@@ -9248,7 +9564,7 @@
         <v>4.9395829100104498</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7">
       <c r="A206" s="40">
         <v>71</v>
       </c>
@@ -9271,7 +9587,7 @@
         <v>4.9862213585230597</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7">
       <c r="A207" s="40">
         <v>70</v>
       </c>
@@ -9294,7 +9610,7 @@
         <v>4.9439126321571996</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7">
       <c r="A208" s="40">
         <v>57</v>
       </c>
@@ -9317,7 +9633,7 @@
         <v>4.9849030384514199</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7">
       <c r="A209" s="40">
         <v>34</v>
       </c>
@@ -9340,7 +9656,7 @@
         <v>4.9068183482371097</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7">
       <c r="A210" s="40">
         <v>46</v>
       </c>
@@ -9363,7 +9679,7 @@
         <v>4.8769247345170399</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7">
       <c r="A211" s="40">
         <v>50</v>
       </c>
@@ -9386,7 +9702,7 @@
         <v>4.9009368209212498</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7">
       <c r="A212" s="40">
         <v>42</v>
       </c>
@@ -9409,7 +9725,7 @@
         <v>4.9012714192428302</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7">
       <c r="A213" s="40">
         <v>13</v>
       </c>
@@ -9432,7 +9748,7 @@
         <v>4.9020901290299799</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7">
       <c r="A214" s="40">
         <v>8</v>
       </c>
@@ -9455,7 +9771,7 @@
         <v>4.8966468783883403</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7">
       <c r="A215" s="40">
         <v>52</v>
       </c>
@@ -9478,7 +9794,7 @@
         <v>4.9323732780000196</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7">
       <c r="A216" s="40">
         <v>31</v>
       </c>
@@ -9501,7 +9817,7 @@
         <v>4.8801200401468998</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7">
       <c r="A217" s="40">
         <v>12</v>
       </c>
@@ -9524,7 +9840,7 @@
         <v>4.9138020842507304</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7">
       <c r="A218" s="40">
         <v>194</v>
       </c>
@@ -9547,7 +9863,7 @@
         <v>4.8976672835590804</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7">
       <c r="A219" s="40">
         <v>63</v>
       </c>
@@ -9570,7 +9886,7 @@
         <v>4.8308578794968096</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7">
       <c r="A220" s="40">
         <v>85</v>
       </c>
@@ -9593,7 +9909,7 @@
         <v>4.9672718063421</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7">
       <c r="A221" s="40">
         <v>95</v>
       </c>
@@ -9616,7 +9932,7 @@
         <v>4.9651598465625399</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7">
       <c r="A222" s="40">
         <v>205</v>
       </c>
@@ -9639,7 +9955,7 @@
         <v>4.9003741594096697</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7">
       <c r="A223" s="40">
         <v>28</v>
       </c>
@@ -9662,7 +9978,7 @@
         <v>4.8534977498145198</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7">
       <c r="A224" s="40">
         <v>217</v>
       </c>
@@ -9685,7 +10001,7 @@
         <v>4.8787088205532099</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7">
       <c r="A225" s="40">
         <v>9</v>
       </c>
@@ -9708,7 +10024,7 @@
         <v>4.9238701518581998</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7">
       <c r="A226" s="40">
         <v>4</v>
       </c>
@@ -9731,7 +10047,7 @@
         <v>4.9212958750525404</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7">
       <c r="A227" s="40">
         <v>5</v>
       </c>
@@ -9754,7 +10070,7 @@
         <v>4.9015146831223904</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7">
       <c r="A228" s="40">
         <v>11</v>
       </c>
@@ -9777,7 +10093,7 @@
         <v>4.8908396467347099</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7">
       <c r="A229" s="40">
         <v>29</v>
       </c>
@@ -9800,7 +10116,7 @@
         <v>4.8455305658151104</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7">
       <c r="A230" s="40">
         <v>48</v>
       </c>
@@ -9823,7 +10139,7 @@
         <v>4.8716743964329403</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7">
       <c r="A231" s="40">
         <v>60</v>
       </c>
@@ -9846,7 +10162,7 @@
         <v>4.81050451020909</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7">
       <c r="A232" s="40">
         <v>36</v>
       </c>
@@ -9869,7 +10185,7 @@
         <v>4.8662915416849497</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7">
       <c r="A233" s="40">
         <v>51</v>
       </c>
@@ -9892,7 +10208,7 @@
         <v>4.8657323023485102</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7">
       <c r="A234" s="40">
         <v>35</v>
       </c>
@@ -9915,7 +10231,7 @@
         <v>4.8270985860528501</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7">
       <c r="A235" s="40">
         <v>44</v>
       </c>
@@ -9938,7 +10254,7 @@
         <v>4.8866603611553803</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7">
       <c r="A236" s="40">
         <v>47</v>
       </c>
@@ -9961,7 +10277,7 @@
         <v>4.8397249290690896</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7">
       <c r="A237" s="40">
         <v>49</v>
       </c>
@@ -9984,7 +10300,7 @@
         <v>4.8976154183182903</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7">
       <c r="A238" s="40">
         <v>41</v>
       </c>
@@ -10007,7 +10323,7 @@
         <v>4.7987884898221402</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7">
       <c r="A239" s="40">
         <v>38</v>
       </c>
@@ -10030,7 +10346,7 @@
         <v>4.8042462958371104</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7">
       <c r="A240" s="40">
         <v>27</v>
       </c>
@@ -10053,7 +10369,7 @@
         <v>4.74292604653417</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7">
       <c r="A241" s="40">
         <v>125</v>
       </c>
@@ -10076,7 +10392,7 @@
         <v>4.81735433605723</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7">
       <c r="A242" s="40">
         <v>112</v>
       </c>
@@ -10099,7 +10415,7 @@
         <v>4.6565774742667401</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7">
       <c r="A243" s="40">
         <v>130</v>
       </c>
@@ -10122,7 +10438,7 @@
         <v>4.8126833148488801</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7">
       <c r="A244" s="40">
         <v>131</v>
       </c>
@@ -10145,7 +10461,7 @@
         <v>4.7572779230440396</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7">
       <c r="A245" s="40">
         <v>108</v>
       </c>
@@ -10168,7 +10484,7 @@
         <v>4.7293566843745403</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7">
       <c r="A246" s="40">
         <v>122</v>
       </c>
@@ -10191,7 +10507,7 @@
         <v>4.7931099323030102</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7">
       <c r="A247" s="40">
         <v>132</v>
       </c>
@@ -10214,7 +10530,7 @@
         <v>4.74132067848742</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7">
       <c r="A248" s="40">
         <v>109</v>
       </c>
@@ -10237,7 +10553,7 @@
         <v>4.7643787660637402</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7">
       <c r="A249" s="40">
         <v>126</v>
       </c>
@@ -10260,7 +10576,7 @@
         <v>4.7356285355494601</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7">
       <c r="A250" s="40">
         <v>231</v>
       </c>
@@ -10283,7 +10599,7 @@
         <v>4.6819189072321503</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7">
       <c r="A251" s="40">
         <v>137</v>
       </c>
@@ -10306,7 +10622,7 @@
         <v>4.6572240555378004</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7">
       <c r="A252" s="40">
         <v>150</v>
       </c>
@@ -10329,7 +10645,7 @@
         <v>4.6526715037152897</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7">
       <c r="A253" s="40">
         <v>135</v>
       </c>
@@ -10366,24 +10682,24 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.8984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.09765625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:4" ht="14.85" customHeight="1">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-    </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -10397,11 +10713,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:4" ht="98.45" customHeight="1">
+      <c r="A3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="49" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -10411,9 +10727,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="46" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="47"/>
+    <row r="4" spans="1:4" ht="45">
+      <c r="A4" s="47"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
@@ -10421,9 +10737,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="48"/>
+    <row r="5" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A5" s="47"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
@@ -10431,9 +10747,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="115" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
-      <c r="B6" s="49" t="s">
+    <row r="6" spans="1:4" ht="112.5">
+      <c r="A6" s="47"/>
+      <c r="B6" s="52" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -10443,9 +10759,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
+    <row r="7" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -10453,11 +10769,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="230" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:4" ht="225">
+      <c r="A8" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="53" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -10467,9 +10783,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="47"/>
+    <row r="9" spans="1:4" ht="56.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
@@ -10477,9 +10793,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
-      <c r="B10" s="48"/>
+    <row r="10" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A10" s="48"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
@@ -10487,7 +10803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
@@ -10510,24 +10826,24 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.09765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.09765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:4" ht="15.95" customHeight="1">
+      <c r="A1" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.85" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -10541,11 +10857,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="216" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:4" ht="216">
+      <c r="A3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="58" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -10555,9 +10871,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="56"/>
+    <row r="4" spans="1:4" ht="72">
+      <c r="A4" s="56"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="15" t="s">
         <v>33</v>
       </c>
@@ -10565,9 +10881,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="57"/>
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A5" s="57"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="17" t="s">
         <v>35</v>
       </c>
@@ -10575,11 +10891,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="180" x14ac:dyDescent="0.3">
-      <c r="A6" s="52" t="s">
+    <row r="6" spans="1:4" ht="180">
+      <c r="A6" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="58" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -10589,9 +10905,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="56"/>
+    <row r="7" spans="1:4" ht="60">
+      <c r="A7" s="56"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="15" t="s">
         <v>33</v>
       </c>
@@ -10599,9 +10915,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53"/>
-      <c r="B8" s="57"/>
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A8" s="56"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="18" t="s">
         <v>40</v>
       </c>
@@ -10609,9 +10925,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
-      <c r="B9" s="58" t="s">
+    <row r="9" spans="1:4" ht="72">
+      <c r="A9" s="56"/>
+      <c r="B9" s="61" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -10621,9 +10937,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="59"/>
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A10" s="57"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="18" t="s">
         <v>33</v>
       </c>
@@ -10631,7 +10947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
@@ -10654,24 +10970,24 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="67.09765625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="67.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-    </row>
-    <row r="2" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:4" ht="12.95" customHeight="1">
       <c r="A2" s="20" t="s">
         <v>45</v>
       </c>
@@ -10685,11 +11001,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="252" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+    <row r="3" spans="1:4" ht="270">
+      <c r="A3" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="66" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -10699,9 +11015,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A4" s="66"/>
-      <c r="B4" s="68"/>
+    <row r="4" spans="1:4" ht="45">
+      <c r="A4" s="69"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="24" t="s">
         <v>53</v>
       </c>
@@ -10709,9 +11025,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
-      <c r="B5" s="64"/>
+    <row r="5" spans="1:4" ht="12" customHeight="1">
+      <c r="A5" s="70"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="24" t="s">
         <v>55</v>
       </c>
@@ -10719,11 +11035,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="168" x14ac:dyDescent="0.3">
-      <c r="A6" s="65" t="s">
+    <row r="6" spans="1:4" ht="180">
+      <c r="A6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="66" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -10733,9 +11049,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A7" s="66"/>
-      <c r="B7" s="68"/>
+    <row r="7" spans="1:4" ht="45">
+      <c r="A7" s="69"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="24" t="s">
         <v>53</v>
       </c>
@@ -10743,9 +11059,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="67"/>
-      <c r="B8" s="64"/>
+    <row r="8" spans="1:4" ht="12" customHeight="1">
+      <c r="A8" s="70"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="24" t="s">
         <v>61</v>
       </c>
@@ -10753,11 +11069,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="52.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="60" t="s">
+    <row r="9" spans="1:4" ht="56.25">
+      <c r="A9" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="66" t="s">
         <v>64</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -10767,9 +11083,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="A10" s="61"/>
-      <c r="B10" s="64"/>
+    <row r="10" spans="1:4" ht="45">
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="24" t="s">
         <v>67</v>
       </c>
@@ -10777,8 +11093,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
+    <row r="11" spans="1:4" ht="24" customHeight="1">
+      <c r="A11" s="65"/>
       <c r="B11" s="21" t="s">
         <v>58</v>
       </c>
@@ -10789,7 +11105,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A9:A11"/>
@@ -10813,22 +11129,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.3984375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A1" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-    </row>
-    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+    </row>
+    <row r="2" spans="1:3" ht="13.5" customHeight="1">
       <c r="A2" s="27" t="s">
         <v>26</v>
       </c>
@@ -10839,8 +11155,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="161" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:3" ht="161.1" customHeight="1">
+      <c r="A3" s="55" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10850,21 +11166,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53"/>
-      <c r="B4" s="69" t="s">
+    <row r="4" spans="1:3" ht="408.95" customHeight="1">
+      <c r="A4" s="56"/>
+      <c r="B4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="72"/>
-    </row>
-    <row r="6" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="30.2" customHeight="1">
+      <c r="A5" s="57"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="75"/>
+    </row>
+    <row r="6" spans="1:3" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
@@ -10885,22 +11201,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.19921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.3984375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:3" ht="12.95" customHeight="1">
+      <c r="A1" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-    </row>
-    <row r="2" spans="1:3" ht="10.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+    </row>
+    <row r="2" spans="1:3" ht="10.35" customHeight="1">
       <c r="A2" s="29" t="s">
         <v>75</v>
       </c>
@@ -10911,8 +11227,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="66.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:3" ht="66.599999999999994" customHeight="1">
+      <c r="A3" s="77" t="s">
         <v>78</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -10922,8 +11238,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75"/>
+    <row r="4" spans="1:3" ht="24.2" customHeight="1">
+      <c r="A4" s="78"/>
       <c r="B4" s="32" t="s">
         <v>81</v>
       </c>
@@ -10931,8 +11247,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="75"/>
+    <row r="5" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A5" s="78"/>
       <c r="B5" s="30" t="s">
         <v>83</v>
       </c>
@@ -10940,8 +11256,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75"/>
+    <row r="6" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A6" s="78"/>
       <c r="B6" s="30" t="s">
         <v>85</v>
       </c>
@@ -10949,8 +11265,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="75"/>
+    <row r="7" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A7" s="78"/>
       <c r="B7" s="30" t="s">
         <v>87</v>
       </c>
@@ -10958,8 +11274,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
+    <row r="8" spans="1:3" ht="56.25" customHeight="1">
+      <c r="A8" s="78"/>
       <c r="B8" s="30" t="s">
         <v>89</v>
       </c>
@@ -10967,8 +11283,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="76"/>
+    <row r="9" spans="1:3" ht="27.95" customHeight="1">
+      <c r="A9" s="79"/>
       <c r="B9" s="30" t="s">
         <v>91</v>
       </c>
@@ -10976,8 +11292,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="77" t="s">
+    <row r="10" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A10" s="80" t="s">
         <v>93</v>
       </c>
       <c r="B10" s="30" t="s">
@@ -10987,8 +11303,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="70.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
+    <row r="11" spans="1:3" ht="70.349999999999994" customHeight="1">
+      <c r="A11" s="81"/>
       <c r="B11" s="34" t="s">
         <v>96</v>
       </c>
@@ -10996,8 +11312,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="79" t="s">
+    <row r="12" spans="1:3" ht="27.95" customHeight="1">
+      <c r="A12" s="82" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="30" t="s">
@@ -11007,8 +11323,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="80"/>
+    <row r="13" spans="1:3" ht="56.25" customHeight="1">
+      <c r="A13" s="83"/>
       <c r="B13" s="34" t="s">
         <v>96</v>
       </c>
@@ -11016,8 +11332,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
+    <row r="14" spans="1:3" ht="98.25" customHeight="1">
+      <c r="A14" s="84"/>
       <c r="B14" s="34" t="s">
         <v>79</v>
       </c>
@@ -11025,7 +11341,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="24.2" customHeight="1">
       <c r="A15" s="35" t="s">
         <v>102</v>
       </c>
@@ -11036,7 +11352,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
@@ -11057,22 +11373,22 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.69921875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A1" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-    </row>
-    <row r="2" spans="1:3" ht="13.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+    </row>
+    <row r="2" spans="1:3" ht="13.35" customHeight="1">
       <c r="A2" s="36" t="s">
         <v>105</v>
       </c>
@@ -11083,8 +11399,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="83" t="s">
+    <row r="3" spans="1:3" ht="14.85" customHeight="1">
+      <c r="A3" s="86" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -11094,8 +11410,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="84"/>
+    <row r="4" spans="1:3" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="87"/>
       <c r="B4" s="37" t="s">
         <v>111</v>
       </c>
@@ -11103,8 +11419,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="84"/>
+    <row r="5" spans="1:3" ht="22.35" customHeight="1">
+      <c r="A5" s="87"/>
       <c r="B5" s="37" t="s">
         <v>113</v>
       </c>
@@ -11112,8 +11428,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="84"/>
+    <row r="6" spans="1:3" ht="14.85" customHeight="1">
+      <c r="A6" s="87"/>
       <c r="B6" s="37" t="s">
         <v>115</v>
       </c>
@@ -11121,8 +11437,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="84"/>
+    <row r="7" spans="1:3" ht="14.85" customHeight="1">
+      <c r="A7" s="87"/>
       <c r="B7" s="37" t="s">
         <v>117</v>
       </c>
@@ -11130,8 +11446,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
+    <row r="8" spans="1:3" ht="14.85" customHeight="1">
+      <c r="A8" s="88"/>
       <c r="B8" s="37" t="s">
         <v>119</v>
       </c>
@@ -11139,7 +11455,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.85" customHeight="1">
       <c r="A9" s="36" t="s">
         <v>121</v>
       </c>
@@ -11150,7 +11466,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.85" customHeight="1">
       <c r="A10" s="36" t="s">
         <v>123</v>
       </c>
@@ -11161,7 +11477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.85" customHeight="1">
       <c r="A11" s="36" t="s">
         <v>125</v>
       </c>
@@ -11172,14 +11488,14 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86" t="s">
+    <row r="12" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A12" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-    </row>
-    <row r="13" spans="1:3" ht="13.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="89"/>
+      <c r="C12" s="89"/>
+    </row>
+    <row r="13" spans="1:3" ht="13.35" customHeight="1">
       <c r="A13" s="21" t="s">
         <v>46</v>
       </c>
@@ -11190,7 +11506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="26.45" customHeight="1">
       <c r="A14" s="21" t="s">
         <v>64</v>
       </c>
@@ -11201,14 +11517,14 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="86" t="s">
+    <row r="15" spans="1:3" ht="14.1" customHeight="1">
+      <c r="A15" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.25" customHeight="1">
       <c r="A16" s="21" t="s">
         <v>46</v>
       </c>
@@ -11219,7 +11535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.5" customHeight="1">
       <c r="A17" s="21" t="s">
         <v>64</v>
       </c>
@@ -11230,7 +11546,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:3" ht="17.100000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
fix data input error
1 location of school is wrongly recorded
</commit_message>
<xml_diff>
--- a/data/school listing.xlsx
+++ b/data/school listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pre-U\BN_UBD\4. SM2302_Software\git_test\grp-the-r-ones\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875B348C-1DF5-4B60-97B5-1A1FCEBDFCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E793B-2365-426B-A67D-F8A3197FD8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5A9532B9-1078-4A7A-974D-4A0853E75333}"/>
   </bookViews>
@@ -2206,14 +2206,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2480,270 +2487,271 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="12"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="10"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3454,10 +3462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED54A88-6810-4FBE-8CDE-8EA5829FFAA6}">
-  <dimension ref="A1:G253"/>
+  <dimension ref="A1:H253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="J236" sqref="J236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3507,10 +3515,10 @@
       <c r="E2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="90">
+      <c r="F2" s="45">
         <v>114.897315950848</v>
       </c>
-      <c r="G2" s="90">
+      <c r="G2" s="45">
         <v>4.8788501040970198</v>
       </c>
     </row>
@@ -3530,10 +3538,10 @@
       <c r="E3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="90">
+      <c r="F3" s="45">
         <v>114.91324478338301</v>
       </c>
-      <c r="G3" s="90">
+      <c r="G3" s="45">
         <v>4.8923250720796698</v>
       </c>
     </row>
@@ -3553,10 +3561,10 @@
       <c r="E4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="90">
+      <c r="F4" s="45">
         <v>114.900521863305</v>
       </c>
-      <c r="G4" s="90">
+      <c r="G4" s="45">
         <v>4.8983539128464004</v>
       </c>
     </row>
@@ -3576,10 +3584,10 @@
       <c r="E5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="90">
+      <c r="F5" s="45">
         <v>114.88354634900401</v>
       </c>
-      <c r="G5" s="90">
+      <c r="G5" s="45">
         <v>4.9212958750525404</v>
       </c>
     </row>
@@ -3599,10 +3607,10 @@
       <c r="E6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="90">
+      <c r="F6" s="45">
         <v>114.87883878024</v>
       </c>
-      <c r="G6" s="90">
+      <c r="G6" s="45">
         <v>4.9015146831223904</v>
       </c>
     </row>
@@ -3622,10 +3630,10 @@
       <c r="E7" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="90">
+      <c r="F7" s="45">
         <v>114.884798410369</v>
       </c>
-      <c r="G7" s="90">
+      <c r="G7" s="45">
         <v>4.9023086805644001</v>
       </c>
     </row>
@@ -3645,10 +3653,10 @@
       <c r="E8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="90">
+      <c r="F8" s="45">
         <v>114.95554674400501</v>
       </c>
-      <c r="G8" s="90">
+      <c r="G8" s="45">
         <v>4.87249923415777</v>
       </c>
     </row>
@@ -3668,10 +3676,10 @@
       <c r="E9" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="90">
+      <c r="F9" s="45">
         <v>114.935756553716</v>
       </c>
-      <c r="G9" s="90">
+      <c r="G9" s="45">
         <v>4.8966468783883403</v>
       </c>
     </row>
@@ -3691,10 +3699,10 @@
       <c r="E10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="90">
+      <c r="F10" s="45">
         <v>114.886184369313</v>
       </c>
-      <c r="G10" s="90">
+      <c r="G10" s="45">
         <v>4.9238701518581998</v>
       </c>
     </row>
@@ -3714,10 +3722,10 @@
       <c r="E11" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="90">
+      <c r="F11" s="45">
         <v>114.938186841128</v>
       </c>
-      <c r="G11" s="90">
+      <c r="G11" s="45">
         <v>4.8995986234787097</v>
       </c>
     </row>
@@ -3737,10 +3745,10 @@
       <c r="E12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="90">
+      <c r="F12" s="45">
         <v>114.875293688683</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="45">
         <v>4.8908396467347099</v>
       </c>
     </row>
@@ -3760,10 +3768,10 @@
       <c r="E13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="90">
+      <c r="F13" s="45">
         <v>114.92367768786499</v>
       </c>
-      <c r="G13" s="90">
+      <c r="G13" s="45">
         <v>4.9138020842507304</v>
       </c>
     </row>
@@ -3783,10 +3791,10 @@
       <c r="E14" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="90">
+      <c r="F14" s="45">
         <v>114.936528021379</v>
       </c>
-      <c r="G14" s="90">
+      <c r="G14" s="45">
         <v>4.9020901290299799</v>
       </c>
     </row>
@@ -3806,10 +3814,10 @@
       <c r="E15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="90">
+      <c r="F15" s="45">
         <v>114.913180926995</v>
       </c>
-      <c r="G15" s="90">
+      <c r="G15" s="45">
         <v>4.9027129659408502</v>
       </c>
     </row>
@@ -3829,10 +3837,10 @@
       <c r="E16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="90">
+      <c r="F16" s="45">
         <v>115.10661936128299</v>
       </c>
-      <c r="G16" s="90">
+      <c r="G16" s="45">
         <v>4.6226342411964403</v>
       </c>
     </row>
@@ -3852,10 +3860,10 @@
       <c r="E17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="90">
+      <c r="F17" s="45">
         <v>115.18418145376501</v>
       </c>
-      <c r="G17" s="90">
+      <c r="G17" s="45">
         <v>4.7643813772432102</v>
       </c>
     </row>
@@ -3875,10 +3883,10 @@
       <c r="E18" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="90">
+      <c r="F18" s="45">
         <v>115.130261076157</v>
       </c>
-      <c r="G18" s="90">
+      <c r="G18" s="45">
         <v>4.7303408612861197</v>
       </c>
     </row>
@@ -3898,10 +3906,10 @@
       <c r="E19" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="90">
+      <c r="F19" s="45">
         <v>115.045908494418</v>
       </c>
-      <c r="G19" s="90">
+      <c r="G19" s="45">
         <v>4.6984751109092997</v>
       </c>
     </row>
@@ -3921,10 +3929,10 @@
       <c r="E20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="90">
+      <c r="F20" s="45">
         <v>115.06599514716901</v>
       </c>
-      <c r="G20" s="90">
+      <c r="G20" s="45">
         <v>4.6579606885782203</v>
       </c>
     </row>
@@ -3944,10 +3952,10 @@
       <c r="E21" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="90">
+      <c r="F21" s="45">
         <v>115.097352911565</v>
       </c>
-      <c r="G21" s="90">
+      <c r="G21" s="45">
         <v>4.6445794163208296</v>
       </c>
     </row>
@@ -3967,10 +3975,10 @@
       <c r="E22" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="90">
+      <c r="F22" s="45">
         <v>115.19800265389399</v>
       </c>
-      <c r="G22" s="90">
+      <c r="G22" s="45">
         <v>4.67620325092809</v>
       </c>
     </row>
@@ -3990,10 +3998,10 @@
       <c r="E23" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="90">
+      <c r="F23" s="45">
         <v>115.074425440833</v>
       </c>
-      <c r="G23" s="90">
+      <c r="G23" s="45">
         <v>4.56786932643762</v>
       </c>
     </row>
@@ -4013,10 +4021,10 @@
       <c r="E24" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="90">
+      <c r="F24" s="45">
         <v>115.1091086404</v>
       </c>
-      <c r="G24" s="90">
+      <c r="G24" s="45">
         <v>4.7165201229251101</v>
       </c>
     </row>
@@ -4036,10 +4044,10 @@
       <c r="E25" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="90">
+      <c r="F25" s="45">
         <v>115.070435297694</v>
       </c>
-      <c r="G25" s="90">
+      <c r="G25" s="45">
         <v>4.7092599719366799</v>
       </c>
     </row>
@@ -4059,10 +4067,10 @@
       <c r="E26" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="90">
+      <c r="F26" s="45">
         <v>115.076223777146</v>
       </c>
-      <c r="G26" s="90">
+      <c r="G26" s="45">
         <v>4.7122173305573503</v>
       </c>
     </row>
@@ -4082,10 +4090,10 @@
       <c r="E27" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="90">
+      <c r="F27" s="45">
         <v>114.812193580882</v>
       </c>
-      <c r="G27" s="90">
+      <c r="G27" s="45">
         <v>4.8678504471997597</v>
       </c>
     </row>
@@ -4105,10 +4113,10 @@
       <c r="E28" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="90">
+      <c r="F28" s="45">
         <v>114.78908880033801</v>
       </c>
-      <c r="G28" s="90">
+      <c r="G28" s="45">
         <v>4.74292604653417</v>
       </c>
     </row>
@@ -4128,10 +4136,10 @@
       <c r="E29" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="90">
+      <c r="F29" s="45">
         <v>114.88813154967799</v>
       </c>
-      <c r="G29" s="90">
+      <c r="G29" s="45">
         <v>4.8534977498145198</v>
       </c>
     </row>
@@ -4151,10 +4159,10 @@
       <c r="E30" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="90">
+      <c r="F30" s="45">
         <v>114.87011651028099</v>
       </c>
-      <c r="G30" s="90">
+      <c r="G30" s="45">
         <v>4.8455305658151104</v>
       </c>
     </row>
@@ -4174,10 +4182,10 @@
       <c r="E31" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="90">
+      <c r="F31" s="45">
         <v>114.929147699448</v>
       </c>
-      <c r="G31" s="90">
+      <c r="G31" s="45">
         <v>4.8941650727478399</v>
       </c>
     </row>
@@ -4197,10 +4205,10 @@
       <c r="E32" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="90">
+      <c r="F32" s="45">
         <v>114.932101751061</v>
       </c>
-      <c r="G32" s="90">
+      <c r="G32" s="45">
         <v>4.8801200401468998</v>
       </c>
     </row>
@@ -4220,10 +4228,10 @@
       <c r="E33" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="90">
+      <c r="F33" s="45">
         <v>114.841225680882</v>
       </c>
-      <c r="G33" s="90">
+      <c r="G33" s="45">
         <v>4.9381056863291901</v>
       </c>
     </row>
@@ -4243,10 +4251,10 @@
       <c r="E34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="90">
+      <c r="F34" s="45">
         <v>114.936416696224</v>
       </c>
-      <c r="G34" s="90">
+      <c r="G34" s="45">
         <v>4.8863321732307297</v>
       </c>
     </row>
@@ -4266,10 +4274,10 @@
       <c r="E35" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="90">
+      <c r="F35" s="45">
         <v>114.938983889871</v>
       </c>
-      <c r="G35" s="90">
+      <c r="G35" s="45">
         <v>4.9068183482371097</v>
       </c>
     </row>
@@ -4289,10 +4297,10 @@
       <c r="E36" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="90">
+      <c r="F36" s="45">
         <v>114.84320118954599</v>
       </c>
-      <c r="G36" s="90">
+      <c r="G36" s="45">
         <v>4.8270985860528501</v>
       </c>
     </row>
@@ -4312,10 +4320,10 @@
       <c r="E37" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="90">
+      <c r="F37" s="45">
         <v>114.846479542042</v>
       </c>
-      <c r="G37" s="90">
+      <c r="G37" s="45">
         <v>4.8662915416849497</v>
       </c>
     </row>
@@ -4335,10 +4343,10 @@
       <c r="E38" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="90">
+      <c r="F38" s="45">
         <v>114.863152194376</v>
       </c>
-      <c r="G38" s="90">
+      <c r="G38" s="45">
         <v>4.8688363272132396</v>
       </c>
     </row>
@@ -4358,10 +4366,10 @@
       <c r="E39" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="90">
+      <c r="F39" s="45">
         <v>114.809130785031</v>
       </c>
-      <c r="G39" s="90">
+      <c r="G39" s="45">
         <v>4.8042462958371104</v>
       </c>
     </row>
@@ -4381,10 +4389,10 @@
       <c r="E40" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="90">
+      <c r="F40" s="45">
         <v>114.81808300971799</v>
       </c>
-      <c r="G40" s="90">
+      <c r="G40" s="45">
         <v>4.7705592370070899</v>
       </c>
     </row>
@@ -4404,10 +4412,10 @@
       <c r="E41" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="90">
+      <c r="F41" s="45">
         <v>114.939689353894</v>
       </c>
-      <c r="G41" s="90">
+      <c r="G41" s="45">
         <v>4.8743952054183604</v>
       </c>
     </row>
@@ -4427,10 +4435,10 @@
       <c r="E42" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="90">
+      <c r="F42" s="45">
         <v>114.832072424534</v>
       </c>
-      <c r="G42" s="90">
+      <c r="G42" s="45">
         <v>4.7987884898221402</v>
       </c>
     </row>
@@ -4450,10 +4458,10 @@
       <c r="E43" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F43" s="90">
+      <c r="F43" s="45">
         <v>114.937699124178</v>
       </c>
-      <c r="G43" s="90">
+      <c r="G43" s="45">
         <v>4.9012714192428302</v>
       </c>
     </row>
@@ -4473,10 +4481,10 @@
       <c r="E44" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F44" s="90">
+      <c r="F44" s="45">
         <v>114.948782902047</v>
       </c>
-      <c r="G44" s="90">
+      <c r="G44" s="45">
         <v>4.8815741237545698</v>
       </c>
     </row>
@@ -4496,10 +4504,10 @@
       <c r="E45" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="90">
+      <c r="F45" s="45">
         <v>114.84174973534</v>
       </c>
-      <c r="G45" s="90">
+      <c r="G45" s="45">
         <v>4.8866603611553803</v>
       </c>
     </row>
@@ -4519,10 +4527,10 @@
       <c r="E46" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F46" s="90">
+      <c r="F46" s="45">
         <v>114.947716169236</v>
       </c>
-      <c r="G46" s="90">
+      <c r="G46" s="45">
         <v>4.87660471513008</v>
       </c>
     </row>
@@ -4542,10 +4550,10 @@
       <c r="E47" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="90">
+      <c r="F47" s="45">
         <v>114.938907850688</v>
       </c>
-      <c r="G47" s="90">
+      <c r="G47" s="45">
         <v>4.8769247345170399</v>
       </c>
     </row>
@@ -4565,10 +4573,10 @@
       <c r="E48" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="90">
+      <c r="F48" s="45">
         <v>114.84124936443</v>
       </c>
-      <c r="G48" s="90">
+      <c r="G48" s="45">
         <v>4.8397249290690896</v>
       </c>
     </row>
@@ -4588,10 +4596,10 @@
       <c r="E49" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="90">
+      <c r="F49" s="45">
         <v>114.855069519496</v>
       </c>
-      <c r="G49" s="90">
+      <c r="G49" s="45">
         <v>4.8716743964329403</v>
       </c>
     </row>
@@ -4611,10 +4619,10 @@
       <c r="E50" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="90">
+      <c r="F50" s="45">
         <v>114.83237122514601</v>
       </c>
-      <c r="G50" s="90">
+      <c r="G50" s="45">
         <v>4.8976154183182903</v>
       </c>
     </row>
@@ -4634,10 +4642,10 @@
       <c r="E51" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F51" s="90">
+      <c r="F51" s="45">
         <v>114.93845303035999</v>
       </c>
-      <c r="G51" s="90">
+      <c r="G51" s="45">
         <v>4.9009368209212498</v>
       </c>
     </row>
@@ -4657,10 +4665,10 @@
       <c r="E52" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="90">
+      <c r="F52" s="45">
         <v>114.84446874703499</v>
       </c>
-      <c r="G52" s="90">
+      <c r="G52" s="45">
         <v>4.8657323023485102</v>
       </c>
     </row>
@@ -4680,10 +4688,10 @@
       <c r="E53" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F53" s="90">
+      <c r="F53" s="45">
         <v>114.93292749289</v>
       </c>
-      <c r="G53" s="90">
+      <c r="G53" s="45">
         <v>4.9323732780000196</v>
       </c>
     </row>
@@ -4703,10 +4711,10 @@
       <c r="E54" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="90">
+      <c r="F54" s="45">
         <v>114.943341701275</v>
       </c>
-      <c r="G54" s="90">
+      <c r="G54" s="45">
         <v>4.9395829100104498</v>
       </c>
     </row>
@@ -4726,10 +4734,10 @@
       <c r="E55" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="90">
+      <c r="F55" s="45">
         <v>114.949828955567</v>
       </c>
-      <c r="G55" s="90">
+      <c r="G55" s="45">
         <v>5.0035337646778597</v>
       </c>
     </row>
@@ -4749,10 +4757,10 @@
       <c r="E56" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="90">
+      <c r="F56" s="45">
         <v>114.972768111565</v>
       </c>
-      <c r="G56" s="90">
+      <c r="G56" s="45">
         <v>4.9869600243316796</v>
       </c>
     </row>
@@ -4772,10 +4780,10 @@
       <c r="E57" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="90">
+      <c r="F57" s="45">
         <v>114.95757160943</v>
       </c>
-      <c r="G57" s="90">
+      <c r="G57" s="45">
         <v>4.9611573668001503</v>
       </c>
     </row>
@@ -4795,10 +4803,10 @@
       <c r="E58" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="90">
+      <c r="F58" s="45">
         <v>114.941035605046</v>
       </c>
-      <c r="G58" s="90">
+      <c r="G58" s="45">
         <v>4.9849030384514199</v>
       </c>
     </row>
@@ -4818,10 +4826,10 @@
       <c r="E59" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F59" s="90">
+      <c r="F59" s="45">
         <v>114.94757646539399</v>
       </c>
-      <c r="G59" s="90">
+      <c r="G59" s="45">
         <v>4.9682935013493399</v>
       </c>
     </row>
@@ -4841,10 +4849,10 @@
       <c r="E60" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="90">
+      <c r="F60" s="45">
         <v>114.957205319256</v>
       </c>
-      <c r="G60" s="90">
+      <c r="G60" s="45">
         <v>4.9476103533575904</v>
       </c>
     </row>
@@ -4864,10 +4872,10 @@
       <c r="E61" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F61" s="90">
+      <c r="F61" s="45">
         <v>114.853126454936</v>
       </c>
-      <c r="G61" s="90">
+      <c r="G61" s="45">
         <v>4.81050451020909</v>
       </c>
     </row>
@@ -4887,10 +4895,10 @@
       <c r="E62" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="90">
+      <c r="F62" s="45">
         <v>114.946673810514</v>
       </c>
-      <c r="G62" s="90">
+      <c r="G62" s="45">
         <v>4.82309208955476</v>
       </c>
     </row>
@@ -4910,10 +4918,10 @@
       <c r="E63" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F63" s="90">
+      <c r="F63" s="45">
         <v>114.96802449445001</v>
       </c>
-      <c r="G63" s="90">
+      <c r="G63" s="45">
         <v>4.9730793963712401</v>
       </c>
     </row>
@@ -4933,10 +4941,10 @@
       <c r="E64" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F64" s="90">
+      <c r="F64" s="45">
         <v>114.91532751889901</v>
       </c>
-      <c r="G64" s="90">
+      <c r="G64" s="45">
         <v>4.8308578794968096</v>
       </c>
     </row>
@@ -4956,10 +4964,10 @@
       <c r="E65" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F65" s="90">
+      <c r="F65" s="45">
         <v>114.979278165439</v>
       </c>
-      <c r="G65" s="90">
+      <c r="G65" s="45">
         <v>4.86328061288798</v>
       </c>
     </row>
@@ -4979,10 +4987,10 @@
       <c r="E66" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="90">
+      <c r="F66" s="45">
         <v>114.937401453894</v>
       </c>
-      <c r="G66" s="90">
+      <c r="G66" s="45">
         <v>4.9951428877935102</v>
       </c>
     </row>
@@ -5002,10 +5010,10 @@
       <c r="E67" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="90">
+      <c r="F67" s="45">
         <v>114.94739050971801</v>
       </c>
-      <c r="G67" s="90">
+      <c r="G67" s="45">
         <v>4.8740388561010999</v>
       </c>
     </row>
@@ -5025,10 +5033,10 @@
       <c r="E68" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="90">
+      <c r="F68" s="45">
         <v>114.96017569991901</v>
       </c>
-      <c r="G68" s="90">
+      <c r="G68" s="45">
         <v>4.9802544683401901</v>
       </c>
     </row>
@@ -5048,10 +5056,10 @@
       <c r="E69" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="90">
+      <c r="F69" s="45">
         <v>114.949837146842</v>
       </c>
-      <c r="G69" s="90">
+      <c r="G69" s="45">
         <v>4.9325702172486201</v>
       </c>
     </row>
@@ -5071,10 +5079,10 @@
       <c r="E70" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F70" s="90">
+      <c r="F70" s="45">
         <v>114.971102324481</v>
       </c>
-      <c r="G70" s="90">
+      <c r="G70" s="45">
         <v>4.8329781069781701</v>
       </c>
     </row>
@@ -5094,10 +5102,10 @@
       <c r="E71" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="90">
+      <c r="F71" s="45">
         <v>114.942095486287</v>
       </c>
-      <c r="G71" s="90">
+      <c r="G71" s="45">
         <v>4.9439126321571996</v>
       </c>
     </row>
@@ -5117,10 +5125,10 @@
       <c r="E72" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="90">
+      <c r="F72" s="45">
         <v>114.942613851389</v>
       </c>
-      <c r="G72" s="90">
+      <c r="G72" s="45">
         <v>4.9862213585230597</v>
       </c>
     </row>
@@ -5140,10 +5148,10 @@
       <c r="E73" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="90">
+      <c r="F73" s="45">
         <v>114.97073764216501</v>
       </c>
-      <c r="G73" s="90">
+      <c r="G73" s="45">
         <v>4.9310816401703104</v>
       </c>
     </row>
@@ -5163,10 +5171,10 @@
       <c r="E74" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="90">
+      <c r="F74" s="45">
         <v>114.970237325059</v>
       </c>
-      <c r="G74" s="90">
+      <c r="G74" s="45">
         <v>4.9823007194873501</v>
       </c>
     </row>
@@ -5186,10 +5194,10 @@
       <c r="E75" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="90">
+      <c r="F75" s="45">
         <v>114.94518897815</v>
       </c>
-      <c r="G75" s="90">
+      <c r="G75" s="45">
         <v>4.8631400434660499</v>
       </c>
     </row>
@@ -5209,10 +5217,10 @@
       <c r="E76" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F76" s="90">
+      <c r="F76" s="45">
         <v>114.954508196052</v>
       </c>
-      <c r="G76" s="90">
+      <c r="G76" s="45">
         <v>4.9295250645260502</v>
       </c>
     </row>
@@ -5232,10 +5240,10 @@
       <c r="E77" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F77" s="90">
+      <c r="F77" s="45">
         <v>114.949631832118</v>
       </c>
-      <c r="G77" s="90">
+      <c r="G77" s="45">
         <v>4.9470109997956904</v>
       </c>
     </row>
@@ -5255,10 +5263,10 @@
       <c r="E78" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F78" s="90">
+      <c r="F78" s="45">
         <v>115.032979583291</v>
       </c>
-      <c r="G78" s="90">
+      <c r="G78" s="45">
         <v>4.9828639927883804</v>
       </c>
     </row>
@@ -5278,10 +5286,10 @@
       <c r="E79" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F79" s="90">
+      <c r="F79" s="45">
         <v>115.028979780882</v>
       </c>
-      <c r="G79" s="90">
+      <c r="G79" s="45">
         <v>4.9687003342927998</v>
       </c>
     </row>
@@ -5301,10 +5309,10 @@
       <c r="E80" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F80" s="90">
+      <c r="F80" s="45">
         <v>114.975559981</v>
       </c>
-      <c r="G80" s="90">
+      <c r="G80" s="45">
         <v>4.9665264546792303</v>
       </c>
     </row>
@@ -5324,10 +5332,10 @@
       <c r="E81" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F81" s="90">
+      <c r="F81" s="45">
         <v>115.04618076320899</v>
       </c>
-      <c r="G81" s="90">
+      <c r="G81" s="45">
         <v>5.0235194825777603</v>
       </c>
     </row>
@@ -5347,10 +5355,10 @@
       <c r="E82" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F82" s="90">
+      <c r="F82" s="45">
         <v>115.020333862084</v>
       </c>
-      <c r="G82" s="90">
+      <c r="G82" s="45">
         <v>4.9725808072562501</v>
       </c>
     </row>
@@ -5370,10 +5378,10 @@
       <c r="E83" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F83" s="90">
+      <c r="F83" s="45">
         <v>114.972926080984</v>
       </c>
-      <c r="G83" s="90">
+      <c r="G83" s="45">
         <v>4.8986274743195404</v>
       </c>
     </row>
@@ -5393,10 +5401,10 @@
       <c r="E84" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F84" s="90">
+      <c r="F84" s="45">
         <v>114.91426752522</v>
       </c>
-      <c r="G84" s="90">
+      <c r="G84" s="45">
         <v>4.9481351660812498</v>
       </c>
     </row>
@@ -5416,10 +5424,10 @@
       <c r="E85" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F85" s="90">
+      <c r="F85" s="45">
         <v>114.90266358266599</v>
       </c>
-      <c r="G85" s="90">
+      <c r="G85" s="45">
         <v>4.9598276543794304</v>
       </c>
     </row>
@@ -5439,10 +5447,10 @@
       <c r="E86" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="90">
+      <c r="F86" s="45">
         <v>114.91325233674699</v>
       </c>
-      <c r="G86" s="90">
+      <c r="G86" s="45">
         <v>4.9672718063421</v>
       </c>
     </row>
@@ -5462,10 +5470,10 @@
       <c r="E87" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="90">
+      <c r="F87" s="45">
         <v>115.05900275620399</v>
       </c>
-      <c r="G87" s="90">
+      <c r="G87" s="45">
         <v>5.0209225218448896</v>
       </c>
     </row>
@@ -5485,10 +5493,10 @@
       <c r="E88" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F88" s="90">
+      <c r="F88" s="45">
         <v>115.02002102700899</v>
       </c>
-      <c r="G88" s="90">
+      <c r="G88" s="45">
         <v>4.9441469528076301</v>
       </c>
     </row>
@@ -5508,10 +5516,10 @@
       <c r="E89" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="90">
+      <c r="F89" s="45">
         <v>115.068229277092</v>
       </c>
-      <c r="G89" s="90">
+      <c r="G89" s="45">
         <v>5.0285621676142203</v>
       </c>
     </row>
@@ -5531,10 +5539,10 @@
       <c r="E90" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F90" s="90">
+      <c r="F90" s="45">
         <v>115.00246183970501</v>
       </c>
-      <c r="G90" s="90">
+      <c r="G90" s="45">
         <v>4.9971881631241502</v>
       </c>
     </row>
@@ -5554,10 +5562,10 @@
       <c r="E91" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F91" s="90">
+      <c r="F91" s="45">
         <v>115.01383510038001</v>
       </c>
-      <c r="G91" s="90">
+      <c r="G91" s="45">
         <v>4.9151194099804902</v>
       </c>
     </row>
@@ -5577,10 +5585,10 @@
       <c r="E92" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F92" s="90">
+      <c r="F92" s="45">
         <v>115.067516348425</v>
       </c>
-      <c r="G92" s="90">
+      <c r="G92" s="45">
         <v>5.0355240870730897</v>
       </c>
     </row>
@@ -5600,10 +5608,10 @@
       <c r="E93" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F93" s="90">
+      <c r="F93" s="45">
         <v>115.026176945694</v>
       </c>
-      <c r="G93" s="90">
+      <c r="G93" s="45">
         <v>4.9666167041530596</v>
       </c>
     </row>
@@ -5623,10 +5631,10 @@
       <c r="E94" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F94" s="90">
+      <c r="F94" s="45">
         <v>115.057911313445</v>
       </c>
-      <c r="G94" s="90">
+      <c r="G94" s="45">
         <v>5.0250068007910604</v>
       </c>
     </row>
@@ -5646,10 +5654,10 @@
       <c r="E95" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F95" s="90">
+      <c r="F95" s="45">
         <v>114.918980249062</v>
       </c>
-      <c r="G95" s="90">
+      <c r="G95" s="45">
         <v>4.95625770436647</v>
       </c>
     </row>
@@ -5669,10 +5677,10 @@
       <c r="E96" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F96" s="90">
+      <c r="F96" s="45">
         <v>114.902070696558</v>
       </c>
-      <c r="G96" s="90">
+      <c r="G96" s="45">
         <v>4.9651598465625399</v>
       </c>
     </row>
@@ -5692,10 +5700,10 @@
       <c r="E97" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F97" s="90">
+      <c r="F97" s="45">
         <v>114.987654821818</v>
       </c>
-      <c r="G97" s="90">
+      <c r="G97" s="45">
         <v>4.9698581976413196</v>
       </c>
     </row>
@@ -5715,10 +5723,10 @@
       <c r="E98" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="90">
+      <c r="F98" s="45">
         <v>115.04125018539899</v>
       </c>
-      <c r="G98" s="90">
+      <c r="G98" s="45">
         <v>5.0360679337986802</v>
       </c>
     </row>
@@ -5738,10 +5746,10 @@
       <c r="E99" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F99" s="90">
+      <c r="F99" s="45">
         <v>114.73228819872099</v>
       </c>
-      <c r="G99" s="90">
+      <c r="G99" s="45">
         <v>4.76842351906045</v>
       </c>
     </row>
@@ -5761,10 +5769,10 @@
       <c r="E100" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F100" s="90">
+      <c r="F100" s="45">
         <v>114.758927940432</v>
       </c>
-      <c r="G100" s="90">
+      <c r="G100" s="45">
         <v>4.7543580088554904</v>
       </c>
     </row>
@@ -5784,10 +5792,10 @@
       <c r="E101" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F101" s="90">
+      <c r="F101" s="45">
         <v>114.757483654108</v>
       </c>
-      <c r="G101" s="90">
+      <c r="G101" s="45">
         <v>4.7834311442014803</v>
       </c>
     </row>
@@ -5807,10 +5815,10 @@
       <c r="E102" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F102" s="90">
+      <c r="F102" s="45">
         <v>114.737334312865</v>
       </c>
-      <c r="G102" s="90">
+      <c r="G102" s="45">
         <v>4.7444934447591498</v>
       </c>
     </row>
@@ -5830,10 +5838,10 @@
       <c r="E103" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F103" s="90">
+      <c r="F103" s="45">
         <v>114.7953567271</v>
       </c>
-      <c r="G103" s="90">
+      <c r="G103" s="45">
         <v>4.8440878901693099</v>
       </c>
     </row>
@@ -5853,10 +5861,10 @@
       <c r="E104" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F104" s="90">
+      <c r="F104" s="45">
         <v>114.761219699593</v>
       </c>
-      <c r="G104" s="90">
+      <c r="G104" s="45">
         <v>4.7921700088590997</v>
       </c>
     </row>
@@ -5876,10 +5884,10 @@
       <c r="E105" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F105" s="90">
+      <c r="F105" s="45">
         <v>114.66654345283899</v>
       </c>
-      <c r="G105" s="90">
+      <c r="G105" s="45">
         <v>4.7454455711760497</v>
       </c>
     </row>
@@ -5899,10 +5907,10 @@
       <c r="E106" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F106" s="90">
+      <c r="F106" s="45">
         <v>114.721017307648</v>
       </c>
-      <c r="G106" s="90">
+      <c r="G106" s="45">
         <v>4.5991076608492598</v>
       </c>
     </row>
@@ -5922,10 +5930,10 @@
       <c r="E107" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F107" s="90">
+      <c r="F107" s="45">
         <v>114.69592744155899</v>
       </c>
-      <c r="G107" s="90">
+      <c r="G107" s="45">
         <v>4.84675944808978</v>
       </c>
     </row>
@@ -5945,10 +5953,10 @@
       <c r="E108" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F108" s="90">
+      <c r="F108" s="45">
         <v>114.726950735755</v>
       </c>
-      <c r="G108" s="90">
+      <c r="G108" s="45">
         <v>4.8282676229633603</v>
       </c>
     </row>
@@ -5968,10 +5976,10 @@
       <c r="E109" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F109" s="90">
+      <c r="F109" s="45">
         <v>114.649540327319</v>
       </c>
-      <c r="G109" s="90">
+      <c r="G109" s="45">
         <v>4.7293566843745403</v>
       </c>
     </row>
@@ -5991,10 +5999,10 @@
       <c r="E110" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F110" s="90">
+      <c r="F110" s="45">
         <v>114.588520910615</v>
       </c>
-      <c r="G110" s="90">
+      <c r="G110" s="45">
         <v>4.7643787660637402</v>
       </c>
     </row>
@@ -6014,10 +6022,10 @@
       <c r="E111" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F111" s="90">
+      <c r="F111" s="45">
         <v>114.644622414057</v>
       </c>
-      <c r="G111" s="90">
+      <c r="G111" s="45">
         <v>4.66750079808671</v>
       </c>
     </row>
@@ -6037,10 +6045,10 @@
       <c r="E112" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F112" s="90">
+      <c r="F112" s="45">
         <v>114.624640187094</v>
       </c>
-      <c r="G112" s="90">
+      <c r="G112" s="45">
         <v>4.6000313609192904</v>
       </c>
     </row>
@@ -6060,10 +6068,10 @@
       <c r="E113" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F113" s="90">
+      <c r="F113" s="45">
         <v>114.727128903051</v>
       </c>
-      <c r="G113" s="90">
+      <c r="G113" s="45">
         <v>4.6565774742667401</v>
       </c>
     </row>
@@ -6083,10 +6091,10 @@
       <c r="E114" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F114" s="90">
+      <c r="F114" s="45">
         <v>114.69216387486</v>
       </c>
-      <c r="G114" s="90">
+      <c r="G114" s="45">
         <v>4.8159345377176797</v>
       </c>
     </row>
@@ -6106,10 +6114,10 @@
       <c r="E115" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F115" s="90">
+      <c r="F115" s="45">
         <v>114.72055036765001</v>
       </c>
-      <c r="G115" s="90">
+      <c r="G115" s="45">
         <v>4.6875148950958199</v>
       </c>
     </row>
@@ -6129,10 +6137,10 @@
       <c r="E116" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F116" s="90">
+      <c r="F116" s="45">
         <v>114.663174094002</v>
       </c>
-      <c r="G116" s="90">
+      <c r="G116" s="45">
         <v>4.7648756757216599</v>
       </c>
     </row>
@@ -6152,10 +6160,10 @@
       <c r="E117" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F117" s="90">
+      <c r="F117" s="45">
         <v>114.66064857704001</v>
       </c>
-      <c r="G117" s="90">
+      <c r="G117" s="45">
         <v>4.8087886851641297</v>
       </c>
     </row>
@@ -6175,10 +6183,10 @@
       <c r="E118" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F118" s="90">
+      <c r="F118" s="45">
         <v>114.678147617617</v>
       </c>
-      <c r="G118" s="90">
+      <c r="G118" s="45">
         <v>4.6402900712881401</v>
       </c>
     </row>
@@ -6198,10 +6206,10 @@
       <c r="E119" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F119" s="90">
+      <c r="F119" s="45">
         <v>114.681062264814</v>
       </c>
-      <c r="G119" s="90">
+      <c r="G119" s="45">
         <v>4.8398245652697502</v>
       </c>
     </row>
@@ -6221,10 +6229,10 @@
       <c r="E120" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F120" s="90">
+      <c r="F120" s="45">
         <v>114.66974369709401</v>
       </c>
-      <c r="G120" s="90">
+      <c r="G120" s="45">
         <v>4.7180169443587099</v>
       </c>
     </row>
@@ -6244,10 +6252,10 @@
       <c r="E121" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F121" s="90">
+      <c r="F121" s="45">
         <v>114.64768012670901</v>
       </c>
-      <c r="G121" s="90">
+      <c r="G121" s="45">
         <v>4.8016338157133802</v>
       </c>
     </row>
@@ -6267,10 +6275,10 @@
       <c r="E122" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F122" s="90">
+      <c r="F122" s="45">
         <v>114.611483991104</v>
       </c>
-      <c r="G122" s="90">
+      <c r="G122" s="45">
         <v>4.7377314115201301</v>
       </c>
     </row>
@@ -6290,10 +6298,10 @@
       <c r="E123" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F123" s="90">
+      <c r="F123" s="45">
         <v>114.62380879770301</v>
       </c>
-      <c r="G123" s="90">
+      <c r="G123" s="45">
         <v>4.7931099323030102</v>
       </c>
     </row>
@@ -6313,10 +6321,10 @@
       <c r="E124" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F124" s="90">
+      <c r="F124" s="45">
         <v>114.616663882995</v>
       </c>
-      <c r="G124" s="90">
+      <c r="G124" s="45">
         <v>4.7427102091905597</v>
       </c>
     </row>
@@ -6336,10 +6344,10 @@
       <c r="E125" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F125" s="90">
+      <c r="F125" s="45">
         <v>114.650858060432</v>
       </c>
-      <c r="G125" s="90">
+      <c r="G125" s="45">
         <v>4.6385652883661397</v>
       </c>
     </row>
@@ -6359,10 +6367,10 @@
       <c r="E126" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F126" s="90">
+      <c r="F126" s="45">
         <v>114.745124532048</v>
       </c>
-      <c r="G126" s="90">
+      <c r="G126" s="45">
         <v>4.81735433605723</v>
       </c>
     </row>
@@ -6382,10 +6390,10 @@
       <c r="E127" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F127" s="90">
+      <c r="F127" s="45">
         <v>114.560597057376</v>
       </c>
-      <c r="G127" s="90">
+      <c r="G127" s="45">
         <v>4.7356285355494601</v>
       </c>
     </row>
@@ -6405,10 +6413,10 @@
       <c r="E128" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F128" s="90">
+      <c r="F128" s="45">
         <v>114.66810965408401</v>
       </c>
-      <c r="G128" s="90">
+      <c r="G128" s="45">
         <v>4.8255568011729304</v>
       </c>
     </row>
@@ -6428,10 +6436,10 @@
       <c r="E129" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F129" s="90">
+      <c r="F129" s="45">
         <v>114.664347117308</v>
       </c>
-      <c r="G129" s="90">
+      <c r="G129" s="45">
         <v>4.8183640550390097</v>
       </c>
     </row>
@@ -6451,10 +6459,10 @@
       <c r="E130" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F130" s="90">
+      <c r="F130" s="45">
         <v>114.60892081603301</v>
       </c>
-      <c r="G130" s="90">
+      <c r="G130" s="45">
         <v>4.7370779492505504</v>
       </c>
     </row>
@@ -6474,10 +6482,10 @@
       <c r="E131" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F131" s="90">
+      <c r="F131" s="45">
         <v>114.663995020456</v>
       </c>
-      <c r="G131" s="90">
+      <c r="G131" s="45">
         <v>4.8126833148488801</v>
       </c>
     </row>
@@ -6497,10 +6505,10 @@
       <c r="E132" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F132" s="90">
+      <c r="F132" s="45">
         <v>114.659939657561</v>
       </c>
-      <c r="G132" s="90">
+      <c r="G132" s="45">
         <v>4.7572779230440396</v>
       </c>
     </row>
@@ -6520,10 +6528,10 @@
       <c r="E133" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F133" s="90">
+      <c r="F133" s="45">
         <v>114.604814871052</v>
       </c>
-      <c r="G133" s="90">
+      <c r="G133" s="45">
         <v>4.74132067848742</v>
       </c>
     </row>
@@ -6543,10 +6551,10 @@
       <c r="E134" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F134" s="90">
+      <c r="F134" s="45">
         <v>114.189109368872</v>
       </c>
-      <c r="G134" s="90">
+      <c r="G134" s="45">
         <v>4.5861949630151697</v>
       </c>
     </row>
@@ -6566,10 +6574,10 @@
       <c r="E135" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F135" s="90">
+      <c r="F135" s="45">
         <v>114.624547375863</v>
       </c>
-      <c r="G135" s="90">
+      <c r="G135" s="45">
         <v>4.3109317643032696</v>
       </c>
     </row>
@@ -6589,10 +6597,10 @@
       <c r="E136" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F136" s="90">
+      <c r="F136" s="45">
         <v>114.18929586932801</v>
       </c>
-      <c r="G136" s="90">
+      <c r="G136" s="45">
         <v>4.5875634963549903</v>
       </c>
     </row>
@@ -6612,10 +6620,10 @@
       <c r="E137" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F137" s="90">
+      <c r="F137" s="45">
         <v>114.465065791447</v>
       </c>
-      <c r="G137" s="90">
+      <c r="G137" s="45">
         <v>4.4139990409059102</v>
       </c>
     </row>
@@ -6635,10 +6643,10 @@
       <c r="E138" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F138" s="90">
+      <c r="F138" s="45">
         <v>114.458580500479</v>
       </c>
-      <c r="G138" s="90">
+      <c r="G138" s="45">
         <v>4.6572240555378004</v>
       </c>
     </row>
@@ -6658,10 +6666,10 @@
       <c r="E139" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F139" s="90">
+      <c r="F139" s="45">
         <v>114.658589956944</v>
       </c>
-      <c r="G139" s="90">
+      <c r="G139" s="45">
         <v>4.2585058157698397</v>
       </c>
     </row>
@@ -6681,10 +6689,10 @@
       <c r="E140" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F140" s="90">
+      <c r="F140" s="45">
         <v>114.575036129537</v>
       </c>
-      <c r="G140" s="90">
+      <c r="G140" s="45">
         <v>4.5261428986584997</v>
       </c>
     </row>
@@ -6704,10 +6712,10 @@
       <c r="E141" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F141" s="90">
+      <c r="F141" s="45">
         <v>114.32802288553999</v>
       </c>
-      <c r="G141" s="90">
+      <c r="G141" s="45">
         <v>4.6120030974922797</v>
       </c>
     </row>
@@ -6727,10 +6735,10 @@
       <c r="E142" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F142" s="90">
+      <c r="F142" s="45">
         <v>114.551078617973</v>
       </c>
-      <c r="G142" s="90">
+      <c r="G142" s="45">
         <v>4.5248760880076997</v>
       </c>
     </row>
@@ -6750,10 +6758,10 @@
       <c r="E143" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F143" s="90">
+      <c r="F143" s="45">
         <v>115.068248005459</v>
       </c>
-      <c r="G143" s="90">
+      <c r="G143" s="45">
         <v>5.0285166657720497</v>
       </c>
     </row>
@@ -6773,10 +6781,10 @@
       <c r="E144" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F144" s="90">
+      <c r="F144" s="45">
         <v>114.281746846733</v>
       </c>
-      <c r="G144" s="90">
+      <c r="G144" s="45">
         <v>4.5982388397587899</v>
       </c>
     </row>
@@ -6796,10 +6804,10 @@
       <c r="E145" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F145" s="90">
+      <c r="F145" s="45">
         <v>114.222924093229</v>
       </c>
-      <c r="G145" s="90">
+      <c r="G145" s="45">
         <v>4.58483349757471</v>
       </c>
     </row>
@@ -6819,10 +6827,10 @@
       <c r="E146" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F146" s="90">
+      <c r="F146" s="45">
         <v>114.33174024999499</v>
       </c>
-      <c r="G146" s="90">
+      <c r="G146" s="45">
         <v>4.5964260225702498</v>
       </c>
     </row>
@@ -6842,10 +6850,10 @@
       <c r="E147" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F147" s="90">
+      <c r="F147" s="45">
         <v>114.494956293515</v>
       </c>
-      <c r="G147" s="90">
+      <c r="G147" s="45">
         <v>4.6810751841002496</v>
       </c>
     </row>
@@ -6865,10 +6873,10 @@
       <c r="E148" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F148" s="90">
+      <c r="F148" s="45">
         <v>114.438881381876</v>
       </c>
-      <c r="G148" s="90">
+      <c r="G148" s="45">
         <v>4.6533058386980697</v>
       </c>
     </row>
@@ -6888,10 +6896,10 @@
       <c r="E149" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F149" s="90">
+      <c r="F149" s="45">
         <v>114.178761126057</v>
       </c>
-      <c r="G149" s="90">
+      <c r="G149" s="45">
         <v>4.5885973121300596</v>
       </c>
     </row>
@@ -6911,10 +6919,10 @@
       <c r="E150" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F150" s="90">
+      <c r="F150" s="45">
         <v>114.331139068385</v>
       </c>
-      <c r="G150" s="90">
+      <c r="G150" s="45">
         <v>4.6093643546865097</v>
       </c>
     </row>
@@ -6934,10 +6942,10 @@
       <c r="E151" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F151" s="90">
+      <c r="F151" s="45">
         <v>114.436543163751</v>
       </c>
-      <c r="G151" s="90">
+      <c r="G151" s="45">
         <v>4.6526715037152897</v>
       </c>
     </row>
@@ -6957,10 +6965,10 @@
       <c r="E152" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F152" s="90">
+      <c r="F152" s="45">
         <v>114.20560061946701</v>
       </c>
-      <c r="G152" s="90">
+      <c r="G152" s="45">
         <v>4.5814620889919899</v>
       </c>
     </row>
@@ -6980,10 +6988,10 @@
       <c r="E153" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F153" s="90">
+      <c r="F153" s="45">
         <v>114.22931559536801</v>
       </c>
-      <c r="G153" s="90">
+      <c r="G153" s="45">
         <v>4.5884842733241697</v>
       </c>
     </row>
@@ -7003,10 +7011,10 @@
       <c r="E154" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F154" s="90">
+      <c r="F154" s="45">
         <v>114.24218055674601</v>
       </c>
-      <c r="G154" s="90">
+      <c r="G154" s="45">
         <v>4.5892261897533002</v>
       </c>
     </row>
@@ -7026,10 +7034,10 @@
       <c r="E155" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F155" s="90">
+      <c r="F155" s="45">
         <v>114.810773097221</v>
       </c>
-      <c r="G155" s="90">
+      <c r="G155" s="45">
         <v>4.76510543031136</v>
       </c>
     </row>
@@ -7049,10 +7057,10 @@
       <c r="E156" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F156" s="90">
+      <c r="F156" s="45">
         <v>114.910780139548</v>
       </c>
-      <c r="G156" s="90">
+      <c r="G156" s="45">
         <v>4.9053143440881204</v>
       </c>
     </row>
@@ -7072,10 +7080,10 @@
       <c r="E157" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F157" s="90">
+      <c r="F157" s="45">
         <v>114.880278426057</v>
       </c>
-      <c r="G157" s="90">
+      <c r="G157" s="45">
         <v>4.9412870184547302</v>
       </c>
     </row>
@@ -7095,10 +7103,10 @@
       <c r="E158" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F158" s="90">
+      <c r="F158" s="45">
         <v>114.977481597221</v>
       </c>
-      <c r="G158" s="90">
+      <c r="G158" s="45">
         <v>4.99597604728788</v>
       </c>
     </row>
@@ -7118,10 +7126,10 @@
       <c r="E159" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F159" s="90">
+      <c r="F159" s="45">
         <v>114.95278105489299</v>
       </c>
-      <c r="G159" s="90">
+      <c r="G159" s="45">
         <v>4.9471631054913896</v>
       </c>
     </row>
@@ -7141,10 +7149,10 @@
       <c r="E160" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F160" s="90">
+      <c r="F160" s="45">
         <v>114.933076412565</v>
       </c>
-      <c r="G160" s="90">
+      <c r="G160" s="45">
         <v>4.9050088651079502</v>
       </c>
     </row>
@@ -7164,10 +7172,10 @@
       <c r="E161" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F161" s="90">
+      <c r="F161" s="45">
         <v>114.89394853954801</v>
       </c>
-      <c r="G161" s="90">
+      <c r="G161" s="45">
         <v>4.9729108294122604</v>
       </c>
     </row>
@@ -7187,10 +7195,10 @@
       <c r="E162" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F162" s="90">
+      <c r="F162" s="45">
         <v>114.91246532791</v>
       </c>
-      <c r="G162" s="90">
+      <c r="G162" s="45">
         <v>4.9061572647022604</v>
       </c>
     </row>
@@ -7210,10 +7218,10 @@
       <c r="E163" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F163" s="90">
+      <c r="F163" s="45">
         <v>114.899964112565</v>
       </c>
-      <c r="G163" s="90">
+      <c r="G163" s="45">
         <v>4.9775179206565499</v>
       </c>
     </row>
@@ -7233,10 +7241,10 @@
       <c r="E164" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F164" s="90">
+      <c r="F164" s="45">
         <v>114.205252962427</v>
       </c>
-      <c r="G164" s="90">
+      <c r="G164" s="45">
         <v>4.5791319036699898</v>
       </c>
     </row>
@@ -7256,10 +7264,10 @@
       <c r="E165" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F165" s="90">
+      <c r="F165" s="45">
         <v>114.321692028855</v>
       </c>
-      <c r="G165" s="90">
+      <c r="G165" s="45">
         <v>4.59991565778033</v>
       </c>
     </row>
@@ -7279,10 +7287,10 @@
       <c r="E166" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F166" s="90">
+      <c r="F166" s="45">
         <v>114.899013556746</v>
       </c>
-      <c r="G166" s="90">
+      <c r="G166" s="45">
         <v>4.8734867961035304</v>
       </c>
     </row>
@@ -7302,10 +7310,10 @@
       <c r="E167" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F167" s="90">
+      <c r="F167" s="45">
         <v>114.96261509536799</v>
       </c>
-      <c r="G167" s="90">
+      <c r="G167" s="45">
         <v>4.9286769592548598</v>
       </c>
     </row>
@@ -7325,10 +7333,10 @@
       <c r="E168" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F168" s="90">
+      <c r="F168" s="45">
         <v>114.86170176653199</v>
       </c>
-      <c r="G168" s="90">
+      <c r="G168" s="45">
         <v>4.8861043311774601</v>
       </c>
     </row>
@@ -7348,10 +7356,10 @@
       <c r="E169" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F169" s="90">
+      <c r="F169" s="45">
         <v>115.020341219446</v>
       </c>
-      <c r="G169" s="90">
+      <c r="G169" s="45">
         <v>4.98737969986278</v>
       </c>
     </row>
@@ -7371,10 +7379,10 @@
       <c r="E170" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F170" s="90">
+      <c r="F170" s="45">
         <v>114.925376574335</v>
       </c>
-      <c r="G170" s="90">
+      <c r="G170" s="45">
         <v>4.8954905056637399</v>
       </c>
     </row>
@@ -7394,10 +7402,10 @@
       <c r="E171" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F171" s="90">
+      <c r="F171" s="45">
         <v>114.907229726057</v>
       </c>
-      <c r="G171" s="90">
+      <c r="G171" s="45">
         <v>4.9256807793568704</v>
       </c>
     </row>
@@ -7417,10 +7425,10 @@
       <c r="E172" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F172" s="90">
+      <c r="F172" s="45">
         <v>114.939095570238</v>
       </c>
-      <c r="G172" s="90">
+      <c r="G172" s="45">
         <v>4.90604727053719</v>
       </c>
     </row>
@@ -7440,10 +7448,10 @@
       <c r="E173" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F173" s="90">
+      <c r="F173" s="45">
         <v>114.901726240881</v>
       </c>
-      <c r="G173" s="90">
+      <c r="G173" s="45">
         <v>4.9071816748263997</v>
       </c>
     </row>
@@ -7463,10 +7471,10 @@
       <c r="E174" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F174" s="90">
+      <c r="F174" s="45">
         <v>114.900402395368</v>
       </c>
-      <c r="G174" s="90">
+      <c r="G174" s="45">
         <v>4.9005655289606702</v>
       </c>
     </row>
@@ -7486,10 +7494,10 @@
       <c r="E175" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F175" s="90">
+      <c r="F175" s="45">
         <v>114.97269053164899</v>
       </c>
-      <c r="G175" s="90">
+      <c r="G175" s="45">
         <v>4.9609544543259299</v>
       </c>
     </row>
@@ -7509,10 +7517,10 @@
       <c r="E176" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F176" s="90">
+      <c r="F176" s="45">
         <v>114.83408620149299</v>
       </c>
-      <c r="G176" s="90">
+      <c r="G176" s="45">
         <v>4.9242595945455898</v>
       </c>
     </row>
@@ -7532,10 +7540,10 @@
       <c r="E177" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F177" s="90">
+      <c r="F177" s="45">
         <v>114.955752124204</v>
       </c>
-      <c r="G177" s="90">
+      <c r="G177" s="45">
         <v>4.9510356159267799</v>
       </c>
     </row>
@@ -7555,10 +7563,10 @@
       <c r="E178" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F178" s="90">
+      <c r="F178" s="45">
         <v>114.93171072605701</v>
       </c>
-      <c r="G178" s="90">
+      <c r="G178" s="45">
         <v>4.8952840994274602</v>
       </c>
     </row>
@@ -7578,10 +7586,10 @@
       <c r="E179" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F179" s="90">
+      <c r="F179" s="45">
         <v>115.023354126057</v>
       </c>
-      <c r="G179" s="90">
+      <c r="G179" s="45">
         <v>4.9953121448287199</v>
       </c>
     </row>
@@ -7601,10 +7609,10 @@
       <c r="E180" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F180" s="90">
+      <c r="F180" s="45">
         <v>114.850832410225</v>
       </c>
-      <c r="G180" s="90">
+      <c r="G180" s="45">
         <v>4.8765641954789203</v>
       </c>
     </row>
@@ -7624,10 +7632,10 @@
       <c r="E181" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F181" s="90">
+      <c r="F181" s="45">
         <v>114.962824743255</v>
       </c>
-      <c r="G181" s="90">
+      <c r="G181" s="45">
         <v>4.9256275715587901</v>
       </c>
     </row>
@@ -7647,10 +7655,10 @@
       <c r="E182" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F182" s="90">
+      <c r="F182" s="45">
         <v>114.947763492341</v>
       </c>
-      <c r="G182" s="90">
+      <c r="G182" s="45">
         <v>4.9920162011524001</v>
       </c>
     </row>
@@ -7670,10 +7678,10 @@
       <c r="E183" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F183" s="90">
+      <c r="F183" s="45">
         <v>114.83666459228</v>
       </c>
-      <c r="G183" s="90">
+      <c r="G183" s="45">
         <v>4.9067428211416297</v>
       </c>
     </row>
@@ -7693,10 +7701,10 @@
       <c r="E184" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="90">
+      <c r="F184" s="45">
         <v>114.986053743255</v>
       </c>
-      <c r="G184" s="90">
+      <c r="G184" s="45">
         <v>4.9776438160172303</v>
       </c>
     </row>
@@ -7716,10 +7724,10 @@
       <c r="E185" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F185" s="90">
+      <c r="F185" s="45">
         <v>114.85575885674599</v>
       </c>
-      <c r="G185" s="90">
+      <c r="G185" s="45">
         <v>4.8834337019703398</v>
       </c>
     </row>
@@ -7739,10 +7747,10 @@
       <c r="E186" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F186" s="90">
+      <c r="F186" s="45">
         <v>115.043872768905</v>
       </c>
-      <c r="G186" s="90">
+      <c r="G186" s="45">
         <v>5.0251481345528797</v>
       </c>
     </row>
@@ -7762,10 +7770,10 @@
       <c r="E187" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F187" s="90">
+      <c r="F187" s="45">
         <v>114.942127208339</v>
       </c>
-      <c r="G187" s="90">
+      <c r="G187" s="45">
         <v>4.9384736180992599</v>
       </c>
     </row>
@@ -7785,10 +7793,10 @@
       <c r="E188" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F188" s="90">
+      <c r="F188" s="45">
         <v>114.96481995622599</v>
       </c>
-      <c r="G188" s="90">
+      <c r="G188" s="45">
         <v>4.9469683281091399</v>
       </c>
     </row>
@@ -7808,10 +7816,10 @@
       <c r="E189" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F189" s="90">
+      <c r="F189" s="45">
         <v>114.906574812565</v>
       </c>
-      <c r="G189" s="90">
+      <c r="G189" s="45">
         <v>4.9355857855939798</v>
       </c>
     </row>
@@ -7831,10 +7839,10 @@
       <c r="E190" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F190" s="90">
+      <c r="F190" s="45">
         <v>114.95916722420399</v>
       </c>
-      <c r="G190" s="90">
+      <c r="G190" s="45">
         <v>4.9483650831721198</v>
       </c>
     </row>
@@ -7854,10 +7862,10 @@
       <c r="E191" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F191" s="90">
+      <c r="F191" s="45">
         <v>114.940710110712</v>
       </c>
-      <c r="G191" s="90">
+      <c r="G191" s="45">
         <v>4.9589555119900401</v>
       </c>
     </row>
@@ -7877,10 +7885,10 @@
       <c r="E192" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F192" s="90">
+      <c r="F192" s="45">
         <v>114.948805145107</v>
       </c>
-      <c r="G192" s="90">
+      <c r="G192" s="45">
         <v>4.9354320199706097</v>
       </c>
     </row>
@@ -7900,10 +7908,10 @@
       <c r="E193" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F193" s="90">
+      <c r="F193" s="45">
         <v>114.843592578496</v>
       </c>
-      <c r="G193" s="90">
+      <c r="G193" s="45">
         <v>4.8479260857986599</v>
       </c>
     </row>
@@ -7923,10 +7931,10 @@
       <c r="E194" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F194" s="90">
+      <c r="F194" s="45">
         <v>114.988580332982</v>
       </c>
-      <c r="G194" s="90">
+      <c r="G194" s="45">
         <v>4.9105231536283904</v>
       </c>
     </row>
@@ -7946,10 +7954,10 @@
       <c r="E195" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F195" s="90">
+      <c r="F195" s="45">
         <v>114.916861736257</v>
       </c>
-      <c r="G195" s="90">
+      <c r="G195" s="45">
         <v>4.8976672835590804</v>
       </c>
     </row>
@@ -7969,10 +7977,10 @@
       <c r="E196" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F196" s="90">
+      <c r="F196" s="45">
         <v>114.847673999074</v>
       </c>
-      <c r="G196" s="90">
+      <c r="G196" s="45">
         <v>4.8940362970532396</v>
       </c>
     </row>
@@ -7992,10 +8000,10 @@
       <c r="E197" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F197" s="90">
+      <c r="F197" s="45">
         <v>114.96403735775</v>
       </c>
-      <c r="G197" s="90">
+      <c r="G197" s="45">
         <v>4.94084954947364</v>
       </c>
     </row>
@@ -8015,10 +8023,10 @@
       <c r="E198" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F198" s="90">
+      <c r="F198" s="45">
         <v>114.89072603714</v>
       </c>
-      <c r="G198" s="90">
+      <c r="G198" s="45">
         <v>4.8822144538483796</v>
       </c>
     </row>
@@ -8038,10 +8046,10 @@
       <c r="E199" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F199" s="90">
+      <c r="F199" s="45">
         <v>114.902484804062</v>
       </c>
-      <c r="G199" s="90">
+      <c r="G199" s="45">
         <v>4.9341066639977296</v>
       </c>
     </row>
@@ -8061,10 +8069,10 @@
       <c r="E200" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F200" s="90">
+      <c r="F200" s="45">
         <v>114.93271261015499</v>
       </c>
-      <c r="G200" s="90">
+      <c r="G200" s="45">
         <v>4.92968470825382</v>
       </c>
     </row>
@@ -8084,10 +8092,10 @@
       <c r="E201" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F201" s="90">
+      <c r="F201" s="45">
         <v>114.961600850633</v>
       </c>
-      <c r="G201" s="90">
+      <c r="G201" s="45">
         <v>4.9283333836673604</v>
       </c>
     </row>
@@ -8107,10 +8115,10 @@
       <c r="E202" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F202" s="90">
+      <c r="F202" s="45">
         <v>115.033902346256</v>
       </c>
-      <c r="G202" s="90">
+      <c r="G202" s="45">
         <v>5.0131682780242297</v>
       </c>
     </row>
@@ -8130,10 +8138,10 @@
       <c r="E203" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F203" s="90">
+      <c r="F203" s="45">
         <v>114.982494723648</v>
       </c>
-      <c r="G203" s="90">
+      <c r="G203" s="45">
         <v>4.97682543244147</v>
       </c>
     </row>
@@ -8153,10 +8161,10 @@
       <c r="E204" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F204" s="90">
+      <c r="F204" s="45">
         <v>114.945977760426</v>
       </c>
-      <c r="G204" s="90">
+      <c r="G204" s="45">
         <v>4.9694255192320904</v>
       </c>
     </row>
@@ -8176,10 +8184,10 @@
       <c r="E205" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F205" s="90">
+      <c r="F205" s="45">
         <v>114.963382008305</v>
       </c>
-      <c r="G205" s="90">
+      <c r="G205" s="45">
         <v>4.9618268790267299</v>
       </c>
     </row>
@@ -8199,10 +8207,10 @@
       <c r="E206" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F206" s="90">
+      <c r="F206" s="45">
         <v>114.90045025303</v>
       </c>
-      <c r="G206" s="90">
+      <c r="G206" s="45">
         <v>4.9003741594096697</v>
       </c>
     </row>
@@ -8222,10 +8230,10 @@
       <c r="E207" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F207" s="90">
+      <c r="F207" s="45">
         <v>114.944443123648</v>
       </c>
-      <c r="G207" s="90">
+      <c r="G207" s="45">
         <v>4.8947855790079302</v>
       </c>
     </row>
@@ -8245,10 +8253,10 @@
       <c r="E208" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F208" s="90">
+      <c r="F208" s="45">
         <v>114.937061352483</v>
       </c>
-      <c r="G208" s="90">
+      <c r="G208" s="45">
         <v>4.8964345475109496</v>
       </c>
     </row>
@@ -8268,10 +8276,10 @@
       <c r="E209" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F209" s="90">
+      <c r="F209" s="45">
         <v>114.938948710155</v>
       </c>
-      <c r="G209" s="90">
+      <c r="G209" s="45">
         <v>4.8958303889610102</v>
       </c>
     </row>
@@ -8291,10 +8299,10 @@
       <c r="E210" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F210" s="90">
+      <c r="F210" s="45">
         <v>114.965351179767</v>
       </c>
-      <c r="G210" s="90">
+      <c r="G210" s="45">
         <v>4.9259695013688303</v>
       </c>
     </row>
@@ -8314,10 +8322,10 @@
       <c r="E211" s="40" t="s">
         <v>347</v>
       </c>
-      <c r="F211" s="90">
+      <c r="F211" s="45">
         <v>114.99104853221399</v>
       </c>
-      <c r="G211" s="90">
+      <c r="G211" s="45">
         <v>4.9623238674432102</v>
       </c>
     </row>
@@ -8337,10 +8345,10 @@
       <c r="E212" s="40" t="s">
         <v>347</v>
       </c>
-      <c r="F212" s="90">
+      <c r="F212" s="45">
         <v>114.881493179469</v>
       </c>
-      <c r="G212" s="90">
+      <c r="G212" s="45">
         <v>4.9682628082157798</v>
       </c>
     </row>
@@ -8360,10 +8368,10 @@
       <c r="E213" s="40" t="s">
         <v>350</v>
       </c>
-      <c r="F213" s="90">
+      <c r="F213" s="45">
         <v>114.874788298113</v>
       </c>
-      <c r="G213" s="90">
+      <c r="G213" s="45">
         <v>4.8812206774057598</v>
       </c>
     </row>
@@ -8383,10 +8391,10 @@
       <c r="E214" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F214" s="90">
+      <c r="F214" s="45">
         <v>114.861744679469</v>
       </c>
-      <c r="G214" s="90">
+      <c r="G214" s="45">
         <v>4.8859546733064798</v>
       </c>
     </row>
@@ -8406,10 +8414,10 @@
       <c r="E215" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F215" s="90">
+      <c r="F215" s="45">
         <v>114.900507765149</v>
       </c>
-      <c r="G215" s="90">
+      <c r="G215" s="45">
         <v>4.9004209009387099</v>
       </c>
     </row>
@@ -8429,10 +8437,10 @@
       <c r="E216" s="40" t="s">
         <v>355</v>
       </c>
-      <c r="F216" s="90">
+      <c r="F216" s="45">
         <v>114.92144025248299</v>
       </c>
-      <c r="G216" s="90">
+      <c r="G216" s="45">
         <v>4.9039782385241502</v>
       </c>
     </row>
@@ -8452,10 +8460,10 @@
       <c r="E217" s="40" t="s">
         <v>355</v>
       </c>
-      <c r="F217" s="90">
+      <c r="F217" s="45">
         <v>114.939533694812</v>
       </c>
-      <c r="G217" s="90">
+      <c r="G217" s="45">
         <v>4.9411990405502904</v>
       </c>
     </row>
@@ -8475,10 +8483,10 @@
       <c r="E218" s="40" t="s">
         <v>355</v>
       </c>
-      <c r="F218" s="90">
+      <c r="F218" s="45">
         <v>114.88812020451201</v>
       </c>
-      <c r="G218" s="90">
+      <c r="G218" s="45">
         <v>4.8787088205532099</v>
       </c>
     </row>
@@ -8498,10 +8506,10 @@
       <c r="E219" s="40" t="s">
         <v>355</v>
       </c>
-      <c r="F219" s="90">
+      <c r="F219" s="45">
         <v>114.920302368618</v>
       </c>
-      <c r="G219" s="90">
+      <c r="G219" s="45">
         <v>4.9157430517254399</v>
       </c>
     </row>
@@ -8521,10 +8529,10 @@
       <c r="E220" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F220" s="90">
+      <c r="F220" s="45">
         <v>114.926251188721</v>
       </c>
-      <c r="G220" s="90">
+      <c r="G220" s="45">
         <v>4.9020327077744801</v>
       </c>
     </row>
@@ -8544,10 +8552,10 @@
       <c r="E221" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F221" s="90">
+      <c r="F221" s="45">
         <v>114.932087619405</v>
       </c>
-      <c r="G221" s="90">
+      <c r="G221" s="45">
         <v>4.8859233124276802</v>
       </c>
     </row>
@@ -8567,10 +8575,10 @@
       <c r="E222" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F222" s="90">
+      <c r="F222" s="45">
         <v>114.66062810942999</v>
       </c>
-      <c r="G222" s="90">
+      <c r="G222" s="45">
         <v>4.8171483697024202</v>
       </c>
     </row>
@@ -8590,10 +8598,10 @@
       <c r="E223" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F223" s="90">
+      <c r="F223" s="45">
         <v>114.735647332897</v>
       </c>
-      <c r="G223" s="90">
+      <c r="G223" s="45">
         <v>4.7357562783921798</v>
       </c>
     </row>
@@ -8613,14 +8621,14 @@
       <c r="E224" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F224" s="90">
+      <c r="F224" s="45">
         <v>114.654574091111</v>
       </c>
-      <c r="G224" s="90">
+      <c r="G224" s="45">
         <v>4.80400089518211</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" s="40">
         <v>224</v>
       </c>
@@ -8636,14 +8644,14 @@
       <c r="E225" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F225" s="90">
+      <c r="F225" s="45">
         <v>114.678234721797</v>
       </c>
-      <c r="G225" s="90">
+      <c r="G225" s="45">
         <v>4.8357804332933396</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" s="40">
         <v>225</v>
       </c>
@@ -8659,14 +8667,14 @@
       <c r="E226" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F226" s="90">
+      <c r="F226" s="45">
         <v>114.691941291112</v>
       </c>
-      <c r="G226" s="90">
+      <c r="G226" s="45">
         <v>4.8180393227760598</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" s="40">
         <v>226</v>
       </c>
@@ -8682,14 +8690,14 @@
       <c r="E227" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F227" s="90">
+      <c r="F227" s="45">
         <v>114.65998654824</v>
       </c>
-      <c r="G227" s="90">
+      <c r="G227" s="45">
         <v>4.81828694992927</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" s="40">
         <v>227</v>
       </c>
@@ -8705,14 +8713,14 @@
       <c r="E228" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F228" s="90">
+      <c r="F228" s="45">
         <v>114.263705536454</v>
       </c>
-      <c r="G228" s="90">
+      <c r="G228" s="45">
         <v>4.5931580196447701</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" s="40">
         <v>228</v>
       </c>
@@ -8728,14 +8736,14 @@
       <c r="E229" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="F229" s="90">
+      <c r="F229" s="45">
         <v>114.298008393252</v>
       </c>
-      <c r="G229" s="90">
+      <c r="G229" s="45">
         <v>4.6104012196960502</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" s="40">
         <v>229</v>
       </c>
@@ -8751,14 +8759,14 @@
       <c r="E230" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F230" s="90">
+      <c r="F230" s="45">
         <v>114.475004614092</v>
       </c>
-      <c r="G230" s="90">
+      <c r="G230" s="45">
         <v>4.6296935384779898</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" s="40">
         <v>230</v>
       </c>
@@ -8774,14 +8782,14 @@
       <c r="E231" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F231" s="90">
+      <c r="F231" s="45">
         <v>114.465070401883</v>
       </c>
-      <c r="G231" s="90">
+      <c r="G231" s="45">
         <v>4.4045741591576197</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" s="40">
         <v>231</v>
       </c>
@@ -8797,14 +8805,14 @@
       <c r="E232" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F232" s="90">
+      <c r="F232" s="45">
         <v>114.502964892317</v>
       </c>
-      <c r="G232" s="90">
+      <c r="G232" s="45">
         <v>4.6819189072321503</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" s="40">
         <v>232</v>
       </c>
@@ -8820,14 +8828,14 @@
       <c r="E233" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F233" s="90">
+      <c r="F233" s="45">
         <v>114.946139937635</v>
       </c>
-      <c r="G233" s="90">
+      <c r="G233" s="45">
         <v>4.9690740699832396</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" s="40">
         <v>233</v>
       </c>
@@ -8843,14 +8851,14 @@
       <c r="E234" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F234" s="90">
+      <c r="F234" s="45">
         <v>114.335859047154</v>
       </c>
-      <c r="G234" s="90">
+      <c r="G234" s="45">
         <v>4.6089190670170401</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" s="40">
         <v>234</v>
       </c>
@@ -8866,14 +8874,14 @@
       <c r="E235" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F235" s="90">
+      <c r="F235" s="45">
         <v>114.193432694268</v>
       </c>
-      <c r="G235" s="90">
+      <c r="G235" s="45">
         <v>4.5821046972426798</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" s="40">
         <v>235</v>
       </c>
@@ -8889,14 +8897,14 @@
       <c r="E236" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F236" s="90">
+      <c r="F236" s="45">
         <v>114.27366976358201</v>
       </c>
-      <c r="G236" s="90">
+      <c r="G236" s="45">
         <v>4.5994180154016897</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" s="40">
         <v>236</v>
       </c>
@@ -8912,14 +8920,14 @@
       <c r="E237" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F237" s="90">
+      <c r="F237" s="45">
         <v>114.337973637139</v>
       </c>
-      <c r="G237" s="90">
+      <c r="G237" s="45">
         <v>4.6143039410332101</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" s="40">
         <v>237</v>
       </c>
@@ -8935,14 +8943,15 @@
       <c r="E238" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F238" s="90">
-        <v>114.380217498036</v>
-      </c>
-      <c r="G238" s="90">
-        <v>4.7167398896136001</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F238" s="45">
+        <v>114.19362411303401</v>
+      </c>
+      <c r="G238" s="45">
+        <v>4.5885573095177197</v>
+      </c>
+      <c r="H238" s="46"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" s="40">
         <v>238</v>
       </c>
@@ -8958,14 +8967,14 @@
       <c r="E239" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F239" s="90">
+      <c r="F239" s="45">
         <v>114.31473093563299</v>
       </c>
-      <c r="G239" s="90">
+      <c r="G239" s="45">
         <v>4.6127305621388501</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" s="40">
         <v>239</v>
       </c>
@@ -8981,10 +8990,10 @@
       <c r="E240" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="F240" s="90">
+      <c r="F240" s="45">
         <v>114.335710582625</v>
       </c>
-      <c r="G240" s="90">
+      <c r="G240" s="45">
         <v>4.6098482366727804</v>
       </c>
     </row>
@@ -9004,10 +9013,10 @@
       <c r="E241" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F241" s="90">
+      <c r="F241" s="45">
         <v>115.06073153462199</v>
       </c>
-      <c r="G241" s="90">
+      <c r="G241" s="45">
         <v>4.7026965754013998</v>
       </c>
     </row>
@@ -9027,10 +9036,10 @@
       <c r="E242" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F242" s="90">
+      <c r="F242" s="45">
         <v>115.042643288402</v>
       </c>
-      <c r="G242" s="90">
+      <c r="G242" s="45">
         <v>4.6925738661652696</v>
       </c>
     </row>
@@ -9050,10 +9059,10 @@
       <c r="E243" s="40" t="s">
         <v>350</v>
       </c>
-      <c r="F243" s="90">
+      <c r="F243" s="45">
         <v>114.92926583659801</v>
       </c>
-      <c r="G243" s="90">
+      <c r="G243" s="45">
         <v>4.8841317117683003</v>
       </c>
     </row>
@@ -9073,10 +9082,10 @@
       <c r="E244" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F244" s="90">
+      <c r="F244" s="45">
         <v>114.932310706631</v>
       </c>
-      <c r="G244" s="90">
+      <c r="G244" s="45">
         <v>4.8860279680034102</v>
       </c>
     </row>
@@ -9096,10 +9105,10 @@
       <c r="E245" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F245" s="90">
+      <c r="F245" s="45">
         <v>114.867119192095</v>
       </c>
-      <c r="G245" s="90">
+      <c r="G245" s="45">
         <v>4.9030321558035697</v>
       </c>
     </row>
@@ -9119,10 +9128,10 @@
       <c r="E246" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F246" s="90">
+      <c r="F246" s="45">
         <v>114.929813097249</v>
       </c>
-      <c r="G246" s="90">
+      <c r="G246" s="45">
         <v>4.8823458713999104</v>
       </c>
     </row>
@@ -9142,10 +9151,10 @@
       <c r="E247" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F247" s="90">
+      <c r="F247" s="45">
         <v>114.92749713659801</v>
       </c>
-      <c r="G247" s="90">
+      <c r="G247" s="45">
         <v>4.88731639168829</v>
       </c>
     </row>
@@ -9165,10 +9174,10 @@
       <c r="E248" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="F248" s="90">
+      <c r="F248" s="45">
         <v>114.929270336597</v>
       </c>
-      <c r="G248" s="90">
+      <c r="G248" s="45">
         <v>4.8860237718058501</v>
       </c>
     </row>
@@ -9188,10 +9197,10 @@
       <c r="E249" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F249" s="90">
+      <c r="F249" s="45">
         <v>114.655903509612</v>
       </c>
-      <c r="G249" s="90">
+      <c r="G249" s="45">
         <v>4.8160080595451902</v>
       </c>
     </row>
@@ -9211,10 +9220,10 @@
       <c r="E250" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F250" s="90">
+      <c r="F250" s="45">
         <v>114.229315267282</v>
       </c>
-      <c r="G250" s="90">
+      <c r="G250" s="45">
         <v>4.5808222084550296</v>
       </c>
     </row>
@@ -9234,10 +9243,10 @@
       <c r="E251" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="F251" s="90">
+      <c r="F251" s="45">
         <v>115.069231394268</v>
       </c>
-      <c r="G251" s="90">
+      <c r="G251" s="45">
         <v>4.7089029403794296</v>
       </c>
     </row>
@@ -9257,10 +9266,10 @@
       <c r="E252" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="F252" s="90">
+      <c r="F252" s="45">
         <v>114.981785121599</v>
       </c>
-      <c r="G252" s="90">
+      <c r="G252" s="45">
         <v>4.99217655509214</v>
       </c>
     </row>
@@ -9280,10 +9289,10 @@
       <c r="E253" s="40" t="s">
         <v>394</v>
       </c>
-      <c r="F253" s="90">
+      <c r="F253" s="45">
         <v>114.95035739426901</v>
       </c>
-      <c r="G253" s="90">
+      <c r="G253" s="45">
         <v>4.8854246517403404</v>
       </c>
     </row>
@@ -9315,12 +9324,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -9337,10 +9346,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="51" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -9351,8 +9360,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
@@ -9361,8 +9370,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="51"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
@@ -9371,8 +9380,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="114" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="52" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="54" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -9383,8 +9392,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -9393,10 +9402,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="228" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="55" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -9407,8 +9416,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
@@ -9417,8 +9426,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="10" t="s">
         <v>22</v>
       </c>
@@ -9459,12 +9468,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -9481,10 +9490,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="216" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -9495,8 +9504,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="15" t="s">
         <v>33</v>
       </c>
@@ -9505,8 +9514,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="17" t="s">
         <v>35</v>
       </c>
@@ -9515,10 +9524,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="60" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -9529,8 +9538,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="15" t="s">
         <v>33</v>
       </c>
@@ -9539,8 +9548,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="60"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="18" t="s">
         <v>40</v>
       </c>
@@ -9549,8 +9558,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="61" t="s">
+      <c r="A9" s="58"/>
+      <c r="B9" s="63" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -9561,8 +9570,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="62"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="18" t="s">
         <v>33</v>
       </c>
@@ -9603,12 +9612,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -9625,10 +9634,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="244.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="68" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -9639,8 +9648,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="24" t="s">
         <v>53</v>
       </c>
@@ -9649,8 +9658,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="24" t="s">
         <v>55</v>
       </c>
@@ -9659,10 +9668,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="163.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="68" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -9673,8 +9682,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="71"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="73"/>
       <c r="C7" s="24" t="s">
         <v>53</v>
       </c>
@@ -9683,8 +9692,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="70"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="24" t="s">
         <v>61</v>
       </c>
@@ -9693,10 +9702,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="68" t="s">
         <v>64</v>
       </c>
       <c r="C9" s="22" t="s">
@@ -9707,8 +9716,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="24" t="s">
         <v>67</v>
       </c>
@@ -9717,7 +9726,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="21" t="s">
         <v>58</v>
       </c>
@@ -9761,11 +9770,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -9779,7 +9788,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="161.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -9790,18 +9799,18 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="408.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="72" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="76" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="75"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="77"/>
     </row>
     <row r="6" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -9833,11 +9842,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
     </row>
     <row r="2" spans="1:3" ht="10.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
@@ -9851,7 +9860,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="79" t="s">
         <v>78</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -9862,7 +9871,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="24.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="32" t="s">
         <v>81</v>
       </c>
@@ -9871,7 +9880,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="30" t="s">
         <v>83</v>
       </c>
@@ -9880,7 +9889,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
+      <c r="A6" s="80"/>
       <c r="B6" s="30" t="s">
         <v>85</v>
       </c>
@@ -9889,7 +9898,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="30" t="s">
         <v>87</v>
       </c>
@@ -9898,7 +9907,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78"/>
+      <c r="A8" s="80"/>
       <c r="B8" s="30" t="s">
         <v>89</v>
       </c>
@@ -9907,7 +9916,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="30" t="s">
         <v>91</v>
       </c>
@@ -9916,7 +9925,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="82" t="s">
         <v>93</v>
       </c>
       <c r="B10" s="30" t="s">
@@ -9927,7 +9936,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="70.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="34" t="s">
         <v>96</v>
       </c>
@@ -9936,7 +9945,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="84" t="s">
         <v>98</v>
       </c>
       <c r="B12" s="30" t="s">
@@ -9947,7 +9956,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="34" t="s">
         <v>96</v>
       </c>
@@ -9956,7 +9965,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="84"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="34" t="s">
         <v>79</v>
       </c>
@@ -10005,11 +10014,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
     </row>
     <row r="2" spans="1:3" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
@@ -10023,7 +10032,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="88" t="s">
         <v>108</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -10034,7 +10043,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="37" t="s">
         <v>111</v>
       </c>
@@ -10043,7 +10052,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="37" t="s">
         <v>113</v>
       </c>
@@ -10052,7 +10061,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="37" t="s">
         <v>115</v>
       </c>
@@ -10061,7 +10070,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="37" t="s">
         <v>117</v>
       </c>
@@ -10070,7 +10079,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="37" t="s">
         <v>119</v>
       </c>
@@ -10112,11 +10121,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="91" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="89"/>
-      <c r="C12" s="89"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
     </row>
     <row r="13" spans="1:3" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
@@ -10141,11 +10150,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="91" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
     </row>
     <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">

</xml_diff>